<commit_message>
Atualização de bases das ligas, do dia: 2024-01-29 às 10-56
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -33009,7 +33009,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>5205927</v>
+        <v>5205928</v>
       </c>
       <c r="C366" t="s">
         <v>28</v>
@@ -33021,73 +33021,73 @@
         <v>44821.5</v>
       </c>
       <c r="F366" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G366" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H366">
+        <v>3</v>
+      </c>
+      <c r="I366">
         <v>1</v>
       </c>
-      <c r="I366">
+      <c r="J366" t="s">
+        <v>45</v>
+      </c>
+      <c r="K366">
+        <v>1.666</v>
+      </c>
+      <c r="L366">
         <v>4</v>
       </c>
-      <c r="J366" t="s">
-        <v>46</v>
-      </c>
-      <c r="K366">
-        <v>1.363</v>
-      </c>
-      <c r="L366">
-        <v>5</v>
-      </c>
       <c r="M366">
-        <v>8</v>
+        <v>4.333</v>
       </c>
       <c r="N366">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="O366">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="P366">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q366">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R366">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S366">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T366">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U366">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V366">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W366">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="X366">
         <v>-1</v>
       </c>
       <c r="Y366">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Z366">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA366">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB366">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="AC366">
         <v>-1</v>
@@ -33098,7 +33098,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>5205928</v>
+        <v>5205927</v>
       </c>
       <c r="C367" t="s">
         <v>28</v>
@@ -33110,73 +33110,73 @@
         <v>44821.5</v>
       </c>
       <c r="F367" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G367" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H367">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I367">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J367" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K367">
-        <v>1.666</v>
+        <v>1.363</v>
       </c>
       <c r="L367">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M367">
-        <v>4.333</v>
+        <v>8</v>
       </c>
       <c r="N367">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="O367">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="P367">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q367">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="R367">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="S367">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T367">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U367">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V367">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W367">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X367">
         <v>-1</v>
       </c>
       <c r="Y367">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Z367">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA367">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB367">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
       <c r="AC367">
         <v>-1</v>
@@ -37993,7 +37993,7 @@
         <v>420</v>
       </c>
       <c r="B422">
-        <v>5205973</v>
+        <v>5205971</v>
       </c>
       <c r="C422" t="s">
         <v>28</v>
@@ -38005,76 +38005,76 @@
         <v>44975.54166666666</v>
       </c>
       <c r="F422" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="G422" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H422">
+        <v>0</v>
+      </c>
+      <c r="I422">
+        <v>3</v>
+      </c>
+      <c r="J422" t="s">
+        <v>46</v>
+      </c>
+      <c r="K422">
+        <v>2.2</v>
+      </c>
+      <c r="L422">
+        <v>3.5</v>
+      </c>
+      <c r="M422">
+        <v>3.1</v>
+      </c>
+      <c r="N422">
+        <v>2.55</v>
+      </c>
+      <c r="O422">
+        <v>3.3</v>
+      </c>
+      <c r="P422">
+        <v>2.75</v>
+      </c>
+      <c r="Q422">
+        <v>0</v>
+      </c>
+      <c r="R422">
+        <v>1.85</v>
+      </c>
+      <c r="S422">
+        <v>2</v>
+      </c>
+      <c r="T422">
+        <v>2.5</v>
+      </c>
+      <c r="U422">
+        <v>1.875</v>
+      </c>
+      <c r="V422">
+        <v>1.975</v>
+      </c>
+      <c r="W422">
+        <v>-1</v>
+      </c>
+      <c r="X422">
+        <v>-1</v>
+      </c>
+      <c r="Y422">
+        <v>1.75</v>
+      </c>
+      <c r="Z422">
+        <v>-1</v>
+      </c>
+      <c r="AA422">
         <v>1</v>
       </c>
-      <c r="I422">
-        <v>1</v>
-      </c>
-      <c r="J422" t="s">
-        <v>44</v>
-      </c>
-      <c r="K422">
-        <v>4.75</v>
-      </c>
-      <c r="L422">
-        <v>3.6</v>
-      </c>
-      <c r="M422">
-        <v>1.727</v>
-      </c>
-      <c r="N422">
-        <v>5.75</v>
-      </c>
-      <c r="O422">
-        <v>4.2</v>
-      </c>
-      <c r="P422">
-        <v>1.6</v>
-      </c>
-      <c r="Q422">
-        <v>1</v>
-      </c>
-      <c r="R422">
-        <v>1.825</v>
-      </c>
-      <c r="S422">
-        <v>2.025</v>
-      </c>
-      <c r="T422">
-        <v>2.75</v>
-      </c>
-      <c r="U422">
-        <v>1.925</v>
-      </c>
-      <c r="V422">
-        <v>1.925</v>
-      </c>
-      <c r="W422">
-        <v>-1</v>
-      </c>
-      <c r="X422">
-        <v>3.2</v>
-      </c>
-      <c r="Y422">
-        <v>-1</v>
-      </c>
-      <c r="Z422">
-        <v>0.825</v>
-      </c>
-      <c r="AA422">
-        <v>-1</v>
-      </c>
       <c r="AB422">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AC422">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="423" spans="1:29">
@@ -38082,7 +38082,7 @@
         <v>421</v>
       </c>
       <c r="B423">
-        <v>5205971</v>
+        <v>5205973</v>
       </c>
       <c r="C423" t="s">
         <v>28</v>
@@ -38094,76 +38094,76 @@
         <v>44975.54166666666</v>
       </c>
       <c r="F423" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G423" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H423">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I423">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J423" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K423">
-        <v>2.2</v>
+        <v>4.75</v>
       </c>
       <c r="L423">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M423">
-        <v>3.1</v>
+        <v>1.727</v>
       </c>
       <c r="N423">
-        <v>2.55</v>
+        <v>5.75</v>
       </c>
       <c r="O423">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="P423">
+        <v>1.6</v>
+      </c>
+      <c r="Q423">
+        <v>1</v>
+      </c>
+      <c r="R423">
+        <v>1.825</v>
+      </c>
+      <c r="S423">
+        <v>2.025</v>
+      </c>
+      <c r="T423">
         <v>2.75</v>
       </c>
-      <c r="Q423">
-        <v>0</v>
-      </c>
-      <c r="R423">
-        <v>1.85</v>
-      </c>
-      <c r="S423">
-        <v>2</v>
-      </c>
-      <c r="T423">
-        <v>2.5</v>
-      </c>
       <c r="U423">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V423">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W423">
         <v>-1</v>
       </c>
       <c r="X423">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y423">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z423">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA423">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB423">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AC423">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="424" spans="1:29">
@@ -38171,7 +38171,7 @@
         <v>422</v>
       </c>
       <c r="B424">
-        <v>5205975</v>
+        <v>5207167</v>
       </c>
       <c r="C424" t="s">
         <v>28</v>
@@ -38183,76 +38183,76 @@
         <v>44976.4375</v>
       </c>
       <c r="F424" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G424" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H424">
         <v>1</v>
       </c>
       <c r="I424">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J424" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K424">
-        <v>7</v>
+        <v>3.8</v>
       </c>
       <c r="L424">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M424">
-        <v>1.4</v>
+        <v>1.95</v>
       </c>
       <c r="N424">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="O424">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P424">
-        <v>1.5</v>
+        <v>1.85</v>
       </c>
       <c r="Q424">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R424">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="S424">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="T424">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U424">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V424">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W424">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X424">
         <v>-1</v>
       </c>
       <c r="Y424">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z424">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA424">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB424">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC424">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="425" spans="1:29">
@@ -38260,7 +38260,7 @@
         <v>423</v>
       </c>
       <c r="B425">
-        <v>5207167</v>
+        <v>5205975</v>
       </c>
       <c r="C425" t="s">
         <v>28</v>
@@ -38272,76 +38272,76 @@
         <v>44976.4375</v>
       </c>
       <c r="F425" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G425" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H425">
         <v>1</v>
       </c>
       <c r="I425">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J425" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K425">
-        <v>3.8</v>
+        <v>7</v>
       </c>
       <c r="L425">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="M425">
-        <v>1.95</v>
+        <v>1.4</v>
       </c>
       <c r="N425">
-        <v>4.2</v>
+        <v>6</v>
       </c>
       <c r="O425">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P425">
-        <v>1.85</v>
+        <v>1.5</v>
       </c>
       <c r="Q425">
+        <v>1.25</v>
+      </c>
+      <c r="R425">
+        <v>1.8</v>
+      </c>
+      <c r="S425">
+        <v>2.05</v>
+      </c>
+      <c r="T425">
+        <v>3</v>
+      </c>
+      <c r="U425">
+        <v>1.975</v>
+      </c>
+      <c r="V425">
+        <v>1.875</v>
+      </c>
+      <c r="W425">
+        <v>-1</v>
+      </c>
+      <c r="X425">
+        <v>-1</v>
+      </c>
+      <c r="Y425">
         <v>0.5</v>
       </c>
-      <c r="R425">
-        <v>1.975</v>
-      </c>
-      <c r="S425">
-        <v>1.875</v>
-      </c>
-      <c r="T425">
-        <v>2.5</v>
-      </c>
-      <c r="U425">
-        <v>1.825</v>
-      </c>
-      <c r="V425">
-        <v>2.025</v>
-      </c>
-      <c r="W425">
-        <v>3.2</v>
-      </c>
-      <c r="X425">
-        <v>-1</v>
-      </c>
-      <c r="Y425">
-        <v>-1</v>
-      </c>
       <c r="Z425">
+        <v>-1</v>
+      </c>
+      <c r="AA425">
+        <v>1.05</v>
+      </c>
+      <c r="AB425">
         <v>0.9750000000000001</v>
       </c>
-      <c r="AA425">
-        <v>-1</v>
-      </c>
-      <c r="AB425">
-        <v>-1</v>
-      </c>
       <c r="AC425">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="426" spans="1:29">
@@ -46092,7 +46092,7 @@
         <v>511</v>
       </c>
       <c r="B513">
-        <v>6847027</v>
+        <v>6847026</v>
       </c>
       <c r="C513" t="s">
         <v>28</v>
@@ -46104,73 +46104,73 @@
         <v>45136.5</v>
       </c>
       <c r="F513" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G513" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H513">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I513">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J513" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K513">
         <v>2.1</v>
       </c>
       <c r="L513">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="M513">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="N513">
-        <v>2.3</v>
+        <v>1.833</v>
       </c>
       <c r="O513">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P513">
-        <v>2.8</v>
+        <v>4.2</v>
       </c>
       <c r="Q513">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R513">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="S513">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="T513">
         <v>2.75</v>
       </c>
       <c r="U513">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V513">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W513">
         <v>-1</v>
       </c>
       <c r="X513">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y513">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z513">
         <v>-1</v>
       </c>
       <c r="AA513">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB513">
-        <v>0.825</v>
+        <v>0.925</v>
       </c>
       <c r="AC513">
         <v>-1</v>
@@ -46181,7 +46181,7 @@
         <v>512</v>
       </c>
       <c r="B514">
-        <v>6847026</v>
+        <v>6847027</v>
       </c>
       <c r="C514" t="s">
         <v>28</v>
@@ -46193,73 +46193,73 @@
         <v>45136.5</v>
       </c>
       <c r="F514" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G514" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H514">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I514">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J514" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K514">
         <v>2.1</v>
       </c>
       <c r="L514">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M514">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="N514">
-        <v>1.833</v>
+        <v>2.3</v>
       </c>
       <c r="O514">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P514">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="Q514">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R514">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S514">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="T514">
         <v>2.75</v>
       </c>
       <c r="U514">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V514">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W514">
         <v>-1</v>
       </c>
       <c r="X514">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y514">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z514">
         <v>-1</v>
       </c>
       <c r="AA514">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB514">
-        <v>0.925</v>
+        <v>0.825</v>
       </c>
       <c r="AC514">
         <v>-1</v>
@@ -47783,7 +47783,7 @@
         <v>530</v>
       </c>
       <c r="B532">
-        <v>6847040</v>
+        <v>6846461</v>
       </c>
       <c r="C532" t="s">
         <v>28</v>
@@ -47795,76 +47795,76 @@
         <v>45158.5</v>
       </c>
       <c r="F532" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G532" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H532">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I532">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J532" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K532">
+        <v>9.5</v>
+      </c>
+      <c r="L532">
+        <v>4.8</v>
+      </c>
+      <c r="M532">
+        <v>1.3</v>
+      </c>
+      <c r="N532">
+        <v>5.75</v>
+      </c>
+      <c r="O532">
+        <v>4.2</v>
+      </c>
+      <c r="P532">
+        <v>1.55</v>
+      </c>
+      <c r="Q532">
+        <v>1</v>
+      </c>
+      <c r="R532">
+        <v>1.9</v>
+      </c>
+      <c r="S532">
+        <v>1.95</v>
+      </c>
+      <c r="T532">
+        <v>3</v>
+      </c>
+      <c r="U532">
         <v>1.85</v>
       </c>
-      <c r="L532">
-        <v>3.6</v>
-      </c>
-      <c r="M532">
-        <v>3.8</v>
-      </c>
-      <c r="N532">
-        <v>2</v>
-      </c>
-      <c r="O532">
-        <v>3.4</v>
-      </c>
-      <c r="P532">
-        <v>3.6</v>
-      </c>
-      <c r="Q532">
-        <v>-0.5</v>
-      </c>
-      <c r="R532">
-        <v>2.025</v>
-      </c>
-      <c r="S532">
-        <v>1.825</v>
-      </c>
-      <c r="T532">
-        <v>2.75</v>
-      </c>
-      <c r="U532">
-        <v>1.875</v>
-      </c>
       <c r="V532">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="W532">
         <v>-1</v>
       </c>
       <c r="X532">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y532">
-        <v>-1</v>
+        <v>0.55</v>
       </c>
       <c r="Z532">
         <v>-1</v>
       </c>
       <c r="AA532">
-        <v>0.825</v>
+        <v>0.95</v>
       </c>
       <c r="AB532">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC532">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="533" spans="1:29">
@@ -47872,7 +47872,7 @@
         <v>531</v>
       </c>
       <c r="B533">
-        <v>6846461</v>
+        <v>6851961</v>
       </c>
       <c r="C533" t="s">
         <v>28</v>
@@ -47884,13 +47884,13 @@
         <v>45158.5</v>
       </c>
       <c r="F533" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G533" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H533">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I533">
         <v>5</v>
@@ -47899,58 +47899,58 @@
         <v>46</v>
       </c>
       <c r="K533">
-        <v>9.5</v>
+        <v>4.333</v>
       </c>
       <c r="L533">
-        <v>4.8</v>
+        <v>3.8</v>
       </c>
       <c r="M533">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="N533">
-        <v>5.75</v>
+        <v>3.5</v>
       </c>
       <c r="O533">
-        <v>4.2</v>
+        <v>3.75</v>
       </c>
       <c r="P533">
-        <v>1.55</v>
+        <v>1.95</v>
       </c>
       <c r="Q533">
+        <v>0.5</v>
+      </c>
+      <c r="R533">
+        <v>1.85</v>
+      </c>
+      <c r="S533">
+        <v>2</v>
+      </c>
+      <c r="T533">
+        <v>2.75</v>
+      </c>
+      <c r="U533">
+        <v>1.925</v>
+      </c>
+      <c r="V533">
+        <v>1.925</v>
+      </c>
+      <c r="W533">
+        <v>-1</v>
+      </c>
+      <c r="X533">
+        <v>-1</v>
+      </c>
+      <c r="Y533">
+        <v>0.95</v>
+      </c>
+      <c r="Z533">
+        <v>-1</v>
+      </c>
+      <c r="AA533">
         <v>1</v>
       </c>
-      <c r="R533">
-        <v>1.9</v>
-      </c>
-      <c r="S533">
-        <v>1.95</v>
-      </c>
-      <c r="T533">
-        <v>3</v>
-      </c>
-      <c r="U533">
-        <v>1.85</v>
-      </c>
-      <c r="V533">
-        <v>2</v>
-      </c>
-      <c r="W533">
-        <v>-1</v>
-      </c>
-      <c r="X533">
-        <v>-1</v>
-      </c>
-      <c r="Y533">
-        <v>0.55</v>
-      </c>
-      <c r="Z533">
-        <v>-1</v>
-      </c>
-      <c r="AA533">
-        <v>0.95</v>
-      </c>
       <c r="AB533">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AC533">
         <v>-1</v>
@@ -47961,7 +47961,7 @@
         <v>532</v>
       </c>
       <c r="B534">
-        <v>6851961</v>
+        <v>6847040</v>
       </c>
       <c r="C534" t="s">
         <v>28</v>
@@ -47973,76 +47973,76 @@
         <v>45158.5</v>
       </c>
       <c r="F534" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G534" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H534">
         <v>0</v>
       </c>
       <c r="I534">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J534" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K534">
-        <v>4.333</v>
+        <v>1.85</v>
       </c>
       <c r="L534">
+        <v>3.6</v>
+      </c>
+      <c r="M534">
         <v>3.8</v>
       </c>
-      <c r="M534">
-        <v>1.7</v>
-      </c>
       <c r="N534">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="O534">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P534">
-        <v>1.95</v>
+        <v>3.6</v>
       </c>
       <c r="Q534">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R534">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="S534">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="T534">
         <v>2.75</v>
       </c>
       <c r="U534">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V534">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W534">
         <v>-1</v>
       </c>
       <c r="X534">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y534">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z534">
         <v>-1</v>
       </c>
       <c r="AA534">
-        <v>1</v>
+        <v>0.825</v>
       </c>
       <c r="AB534">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC534">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="535" spans="1:29">
@@ -49919,7 +49919,7 @@
         <v>554</v>
       </c>
       <c r="B556">
-        <v>6847056</v>
+        <v>6847053</v>
       </c>
       <c r="C556" t="s">
         <v>28</v>
@@ -49931,76 +49931,76 @@
         <v>45193.39583333334</v>
       </c>
       <c r="F556" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G556" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H556">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I556">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J556" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K556">
-        <v>3.75</v>
+        <v>1.571</v>
       </c>
       <c r="L556">
-        <v>3.5</v>
+        <v>4.333</v>
       </c>
       <c r="M556">
+        <v>5</v>
+      </c>
+      <c r="N556">
+        <v>1.727</v>
+      </c>
+      <c r="O556">
+        <v>4</v>
+      </c>
+      <c r="P556">
+        <v>4.5</v>
+      </c>
+      <c r="Q556">
+        <v>-0.75</v>
+      </c>
+      <c r="R556">
         <v>1.95</v>
       </c>
-      <c r="N556">
+      <c r="S556">
+        <v>1.9</v>
+      </c>
+      <c r="T556">
+        <v>2.75</v>
+      </c>
+      <c r="U556">
+        <v>1.8</v>
+      </c>
+      <c r="V556">
+        <v>2.05</v>
+      </c>
+      <c r="W556">
+        <v>-1</v>
+      </c>
+      <c r="X556">
         <v>3</v>
       </c>
-      <c r="O556">
-        <v>3.3</v>
-      </c>
-      <c r="P556">
-        <v>2.4</v>
-      </c>
-      <c r="Q556">
-        <v>0</v>
-      </c>
-      <c r="R556">
-        <v>2.1</v>
-      </c>
-      <c r="S556">
-        <v>1.775</v>
-      </c>
-      <c r="T556">
-        <v>2.5</v>
-      </c>
-      <c r="U556">
-        <v>1.925</v>
-      </c>
-      <c r="V556">
-        <v>1.925</v>
-      </c>
-      <c r="W556">
-        <v>2</v>
-      </c>
-      <c r="X556">
-        <v>-1</v>
-      </c>
       <c r="Y556">
         <v>-1</v>
       </c>
       <c r="Z556">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="AA556">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB556">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC556">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="557" spans="1:29">
@@ -50008,7 +50008,7 @@
         <v>555</v>
       </c>
       <c r="B557">
-        <v>6847053</v>
+        <v>6847056</v>
       </c>
       <c r="C557" t="s">
         <v>28</v>
@@ -50020,76 +50020,76 @@
         <v>45193.39583333334</v>
       </c>
       <c r="F557" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G557" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H557">
+        <v>2</v>
+      </c>
+      <c r="I557">
+        <v>1</v>
+      </c>
+      <c r="J557" t="s">
+        <v>45</v>
+      </c>
+      <c r="K557">
+        <v>3.75</v>
+      </c>
+      <c r="L557">
+        <v>3.5</v>
+      </c>
+      <c r="M557">
+        <v>1.95</v>
+      </c>
+      <c r="N557">
+        <v>3</v>
+      </c>
+      <c r="O557">
+        <v>3.3</v>
+      </c>
+      <c r="P557">
+        <v>2.4</v>
+      </c>
+      <c r="Q557">
         <v>0</v>
       </c>
-      <c r="I557">
-        <v>0</v>
-      </c>
-      <c r="J557" t="s">
-        <v>44</v>
-      </c>
-      <c r="K557">
-        <v>1.571</v>
-      </c>
-      <c r="L557">
-        <v>4.333</v>
-      </c>
-      <c r="M557">
-        <v>5</v>
-      </c>
-      <c r="N557">
-        <v>1.727</v>
-      </c>
-      <c r="O557">
-        <v>4</v>
-      </c>
-      <c r="P557">
-        <v>4.5</v>
-      </c>
-      <c r="Q557">
-        <v>-0.75</v>
-      </c>
       <c r="R557">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="S557">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T557">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U557">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V557">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W557">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X557">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y557">
         <v>-1</v>
       </c>
       <c r="Z557">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="AA557">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB557">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC557">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="558" spans="1:29">
@@ -50453,7 +50453,7 @@
         <v>560</v>
       </c>
       <c r="B562">
-        <v>6847061</v>
+        <v>6847060</v>
       </c>
       <c r="C562" t="s">
         <v>28</v>
@@ -50465,61 +50465,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F562" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G562" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H562">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I562">
         <v>0</v>
       </c>
       <c r="J562" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K562">
-        <v>1.909</v>
+        <v>1.25</v>
       </c>
       <c r="L562">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M562">
-        <v>3.9</v>
+        <v>10</v>
       </c>
       <c r="N562">
-        <v>2</v>
+        <v>1.285</v>
       </c>
       <c r="O562">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="P562">
-        <v>3.6</v>
+        <v>9</v>
       </c>
       <c r="Q562">
-        <v>-0.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R562">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="S562">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="T562">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U562">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V562">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W562">
-        <v>-1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="X562">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y562">
         <v>-1</v>
@@ -50528,13 +50528,13 @@
         <v>-1</v>
       </c>
       <c r="AA562">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AB562">
         <v>-1</v>
       </c>
       <c r="AC562">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563" spans="1:29">
@@ -50542,7 +50542,7 @@
         <v>561</v>
       </c>
       <c r="B563">
-        <v>6847060</v>
+        <v>6847061</v>
       </c>
       <c r="C563" t="s">
         <v>28</v>
@@ -50554,61 +50554,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F563" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G563" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H563">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I563">
         <v>0</v>
       </c>
       <c r="J563" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K563">
-        <v>1.25</v>
+        <v>1.909</v>
       </c>
       <c r="L563">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M563">
-        <v>10</v>
+        <v>3.9</v>
       </c>
       <c r="N563">
-        <v>1.285</v>
+        <v>2</v>
       </c>
       <c r="O563">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="P563">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="Q563">
-        <v>-1.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R563">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="S563">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="T563">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U563">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V563">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W563">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X563">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y563">
         <v>-1</v>
@@ -50617,13 +50617,13 @@
         <v>-1</v>
       </c>
       <c r="AA563">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AB563">
         <v>-1</v>
       </c>
       <c r="AC563">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="564" spans="1:29">
@@ -52055,7 +52055,7 @@
         <v>578</v>
       </c>
       <c r="B580">
-        <v>6847070</v>
+        <v>6847073</v>
       </c>
       <c r="C580" t="s">
         <v>28</v>
@@ -52067,46 +52067,46 @@
         <v>45228.4375</v>
       </c>
       <c r="F580" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G580" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H580">
         <v>0</v>
       </c>
       <c r="I580">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J580" t="s">
         <v>46</v>
       </c>
       <c r="K580">
-        <v>1.5</v>
+        <v>3.4</v>
       </c>
       <c r="L580">
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="M580">
-        <v>6</v>
+        <v>1.95</v>
       </c>
       <c r="N580">
-        <v>1.727</v>
+        <v>4.5</v>
       </c>
       <c r="O580">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="P580">
-        <v>4.75</v>
+        <v>1.7</v>
       </c>
       <c r="Q580">
-        <v>-0.75</v>
+        <v>0.75</v>
       </c>
       <c r="R580">
+        <v>1.9</v>
+      </c>
+      <c r="S580">
         <v>1.95</v>
-      </c>
-      <c r="S580">
-        <v>1.9</v>
       </c>
       <c r="T580">
         <v>2.75</v>
@@ -52124,19 +52124,19 @@
         <v>-1</v>
       </c>
       <c r="Y580">
-        <v>3.75</v>
+        <v>0.7</v>
       </c>
       <c r="Z580">
         <v>-1</v>
       </c>
       <c r="AA580">
-        <v>0.8999999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AB580">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AC580">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="581" spans="1:29">
@@ -52144,7 +52144,7 @@
         <v>579</v>
       </c>
       <c r="B581">
-        <v>6847073</v>
+        <v>6847070</v>
       </c>
       <c r="C581" t="s">
         <v>28</v>
@@ -52156,46 +52156,46 @@
         <v>45228.4375</v>
       </c>
       <c r="F581" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G581" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H581">
         <v>0</v>
       </c>
       <c r="I581">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J581" t="s">
         <v>46</v>
       </c>
       <c r="K581">
-        <v>3.4</v>
+        <v>1.5</v>
       </c>
       <c r="L581">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="M581">
+        <v>6</v>
+      </c>
+      <c r="N581">
+        <v>1.727</v>
+      </c>
+      <c r="O581">
+        <v>3.8</v>
+      </c>
+      <c r="P581">
+        <v>4.75</v>
+      </c>
+      <c r="Q581">
+        <v>-0.75</v>
+      </c>
+      <c r="R581">
         <v>1.95</v>
       </c>
-      <c r="N581">
-        <v>4.5</v>
-      </c>
-      <c r="O581">
-        <v>4</v>
-      </c>
-      <c r="P581">
-        <v>1.7</v>
-      </c>
-      <c r="Q581">
-        <v>0.75</v>
-      </c>
-      <c r="R581">
+      <c r="S581">
         <v>1.9</v>
-      </c>
-      <c r="S581">
-        <v>1.95</v>
       </c>
       <c r="T581">
         <v>2.75</v>
@@ -52213,19 +52213,19 @@
         <v>-1</v>
       </c>
       <c r="Y581">
-        <v>0.7</v>
+        <v>3.75</v>
       </c>
       <c r="Z581">
         <v>-1</v>
       </c>
       <c r="AA581">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB581">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AC581">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="582" spans="1:29">
@@ -52411,7 +52411,7 @@
         <v>582</v>
       </c>
       <c r="B584">
-        <v>6847075</v>
+        <v>6847076</v>
       </c>
       <c r="C584" t="s">
         <v>28</v>
@@ -52423,13 +52423,13 @@
         <v>45234.54166666666</v>
       </c>
       <c r="F584" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G584" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H584">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I584">
         <v>0</v>
@@ -52438,43 +52438,43 @@
         <v>45</v>
       </c>
       <c r="K584">
-        <v>2.3</v>
+        <v>1.444</v>
       </c>
       <c r="L584">
-        <v>3.5</v>
+        <v>4.333</v>
       </c>
       <c r="M584">
-        <v>2.875</v>
+        <v>7</v>
       </c>
       <c r="N584">
-        <v>2.1</v>
+        <v>1.285</v>
       </c>
       <c r="O584">
-        <v>3.5</v>
+        <v>5.75</v>
       </c>
       <c r="P584">
-        <v>3.4</v>
+        <v>11</v>
       </c>
       <c r="Q584">
-        <v>-0.25</v>
+        <v>-1.75</v>
       </c>
       <c r="R584">
-        <v>1.775</v>
+        <v>2</v>
       </c>
       <c r="S584">
-        <v>2.1</v>
+        <v>1.85</v>
       </c>
       <c r="T584">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U584">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="V584">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="W584">
-        <v>1.1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="X584">
         <v>-1</v>
@@ -52483,16 +52483,16 @@
         <v>-1</v>
       </c>
       <c r="Z584">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA584">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB584">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC584">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="585" spans="1:29">
@@ -52500,7 +52500,7 @@
         <v>583</v>
       </c>
       <c r="B585">
-        <v>6847076</v>
+        <v>6847075</v>
       </c>
       <c r="C585" t="s">
         <v>28</v>
@@ -52512,13 +52512,13 @@
         <v>45234.54166666666</v>
       </c>
       <c r="F585" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G585" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H585">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I585">
         <v>0</v>
@@ -52527,43 +52527,43 @@
         <v>45</v>
       </c>
       <c r="K585">
-        <v>1.444</v>
+        <v>2.3</v>
       </c>
       <c r="L585">
-        <v>4.333</v>
+        <v>3.5</v>
       </c>
       <c r="M585">
-        <v>7</v>
+        <v>2.875</v>
       </c>
       <c r="N585">
-        <v>1.285</v>
+        <v>2.1</v>
       </c>
       <c r="O585">
-        <v>5.75</v>
+        <v>3.5</v>
       </c>
       <c r="P585">
-        <v>11</v>
+        <v>3.4</v>
       </c>
       <c r="Q585">
-        <v>-1.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R585">
-        <v>2</v>
+        <v>1.775</v>
       </c>
       <c r="S585">
-        <v>1.85</v>
+        <v>2.1</v>
       </c>
       <c r="T585">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U585">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="V585">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="W585">
-        <v>0.2849999999999999</v>
+        <v>1.1</v>
       </c>
       <c r="X585">
         <v>-1</v>
@@ -52572,16 +52572,16 @@
         <v>-1</v>
       </c>
       <c r="Z585">
-        <v>-1</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA585">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB585">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC585">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="586" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-29 às 17-07
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -31674,7 +31674,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>5205913</v>
+        <v>5205914</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31686,40 +31686,40 @@
         <v>44801.5</v>
       </c>
       <c r="F351" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G351" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H351">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I351">
         <v>3</v>
       </c>
       <c r="J351" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K351">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="L351">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M351">
-        <v>2.375</v>
+        <v>2.3</v>
       </c>
       <c r="N351">
-        <v>2.375</v>
+        <v>2.75</v>
       </c>
       <c r="O351">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P351">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="Q351">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R351">
         <v>2.025</v>
@@ -31728,31 +31728,31 @@
         <v>1.825</v>
       </c>
       <c r="T351">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U351">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V351">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="W351">
         <v>-1</v>
       </c>
       <c r="X351">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y351">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z351">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA351">
-        <v>0.825</v>
+        <v>-0</v>
       </c>
       <c r="AB351">
-        <v>0.925</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC351">
         <v>-1</v>
@@ -31763,7 +31763,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>5205914</v>
+        <v>5205915</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31775,73 +31775,73 @@
         <v>44801.5</v>
       </c>
       <c r="F352" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G352" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H352">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I352">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J352" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K352">
-        <v>3</v>
+        <v>2.55</v>
       </c>
       <c r="L352">
         <v>3.4</v>
       </c>
       <c r="M352">
-        <v>2.3</v>
+        <v>2.625</v>
       </c>
       <c r="N352">
-        <v>2.75</v>
+        <v>2.875</v>
       </c>
       <c r="O352">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="P352">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="Q352">
         <v>0</v>
       </c>
       <c r="R352">
+        <v>2.05</v>
+      </c>
+      <c r="S352">
+        <v>1.75</v>
+      </c>
+      <c r="T352">
+        <v>2.5</v>
+      </c>
+      <c r="U352">
+        <v>1.825</v>
+      </c>
+      <c r="V352">
         <v>2.025</v>
       </c>
-      <c r="S352">
-        <v>1.825</v>
-      </c>
-      <c r="T352">
-        <v>2.75</v>
-      </c>
-      <c r="U352">
-        <v>1.975</v>
-      </c>
-      <c r="V352">
-        <v>1.875</v>
-      </c>
       <c r="W352">
         <v>-1</v>
       </c>
       <c r="X352">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y352">
-        <v>-1</v>
+        <v>1.4</v>
       </c>
       <c r="Z352">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA352">
-        <v>-0</v>
+        <v>0.75</v>
       </c>
       <c r="AB352">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AC352">
         <v>-1</v>
@@ -31852,7 +31852,7 @@
         <v>351</v>
       </c>
       <c r="B353">
-        <v>5205915</v>
+        <v>5205913</v>
       </c>
       <c r="C353" t="s">
         <v>28</v>
@@ -31864,55 +31864,55 @@
         <v>44801.5</v>
       </c>
       <c r="F353" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G353" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H353">
         <v>1</v>
       </c>
       <c r="I353">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J353" t="s">
         <v>46</v>
       </c>
       <c r="K353">
-        <v>2.55</v>
+        <v>2.8</v>
       </c>
       <c r="L353">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M353">
-        <v>2.625</v>
+        <v>2.375</v>
       </c>
       <c r="N353">
-        <v>2.875</v>
+        <v>2.375</v>
       </c>
       <c r="O353">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="P353">
-        <v>2.4</v>
+        <v>2.8</v>
       </c>
       <c r="Q353">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R353">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S353">
-        <v>1.75</v>
+        <v>1.825</v>
       </c>
       <c r="T353">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U353">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V353">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W353">
         <v>-1</v>
@@ -31921,16 +31921,16 @@
         <v>-1</v>
       </c>
       <c r="Y353">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="Z353">
         <v>-1</v>
       </c>
       <c r="AA353">
-        <v>0.75</v>
+        <v>0.825</v>
       </c>
       <c r="AB353">
-        <v>0.825</v>
+        <v>0.925</v>
       </c>
       <c r="AC353">
         <v>-1</v>
@@ -33009,7 +33009,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>5205928</v>
+        <v>5205930</v>
       </c>
       <c r="C366" t="s">
         <v>28</v>
@@ -33021,73 +33021,73 @@
         <v>44821.5</v>
       </c>
       <c r="F366" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G366" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H366">
+        <v>1</v>
+      </c>
+      <c r="I366">
+        <v>4</v>
+      </c>
+      <c r="J366" t="s">
+        <v>46</v>
+      </c>
+      <c r="K366">
         <v>3</v>
       </c>
-      <c r="I366">
-        <v>1</v>
-      </c>
-      <c r="J366" t="s">
-        <v>45</v>
-      </c>
-      <c r="K366">
-        <v>1.666</v>
-      </c>
       <c r="L366">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M366">
-        <v>4.333</v>
+        <v>2.2</v>
       </c>
       <c r="N366">
-        <v>1.727</v>
+        <v>2.8</v>
       </c>
       <c r="O366">
-        <v>4.333</v>
+        <v>3.5</v>
       </c>
       <c r="P366">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="Q366">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R366">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="S366">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="T366">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U366">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V366">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="W366">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X366">
         <v>-1</v>
       </c>
       <c r="Y366">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Z366">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA366">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB366">
-        <v>0.925</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC366">
         <v>-1</v>
@@ -33098,7 +33098,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>5205927</v>
+        <v>5205928</v>
       </c>
       <c r="C367" t="s">
         <v>28</v>
@@ -33110,73 +33110,73 @@
         <v>44821.5</v>
       </c>
       <c r="F367" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G367" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H367">
+        <v>3</v>
+      </c>
+      <c r="I367">
         <v>1</v>
       </c>
-      <c r="I367">
+      <c r="J367" t="s">
+        <v>45</v>
+      </c>
+      <c r="K367">
+        <v>1.666</v>
+      </c>
+      <c r="L367">
         <v>4</v>
       </c>
-      <c r="J367" t="s">
-        <v>46</v>
-      </c>
-      <c r="K367">
-        <v>1.363</v>
-      </c>
-      <c r="L367">
-        <v>5</v>
-      </c>
       <c r="M367">
-        <v>8</v>
+        <v>4.333</v>
       </c>
       <c r="N367">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="O367">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="P367">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q367">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R367">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S367">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T367">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U367">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V367">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W367">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="X367">
         <v>-1</v>
       </c>
       <c r="Y367">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Z367">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA367">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB367">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="AC367">
         <v>-1</v>
@@ -33187,7 +33187,7 @@
         <v>366</v>
       </c>
       <c r="B368">
-        <v>5205930</v>
+        <v>5205927</v>
       </c>
       <c r="C368" t="s">
         <v>28</v>
@@ -33199,10 +33199,10 @@
         <v>44821.5</v>
       </c>
       <c r="F368" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G368" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H368">
         <v>1</v>
@@ -33214,40 +33214,40 @@
         <v>46</v>
       </c>
       <c r="K368">
-        <v>3</v>
+        <v>1.363</v>
       </c>
       <c r="L368">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="M368">
-        <v>2.2</v>
+        <v>8</v>
       </c>
       <c r="N368">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O368">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P368">
-        <v>2.375</v>
+        <v>6</v>
       </c>
       <c r="Q368">
-        <v>0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R368">
+        <v>2.05</v>
+      </c>
+      <c r="S368">
         <v>1.8</v>
       </c>
-      <c r="S368">
-        <v>2.05</v>
-      </c>
       <c r="T368">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U368">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V368">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W368">
         <v>-1</v>
@@ -33256,16 +33256,16 @@
         <v>-1</v>
       </c>
       <c r="Y368">
-        <v>1.375</v>
+        <v>5</v>
       </c>
       <c r="Z368">
         <v>-1</v>
       </c>
       <c r="AA368">
-        <v>1.05</v>
+        <v>0.8</v>
       </c>
       <c r="AB368">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AC368">
         <v>-1</v>
@@ -37993,7 +37993,7 @@
         <v>420</v>
       </c>
       <c r="B422">
-        <v>5205971</v>
+        <v>5205973</v>
       </c>
       <c r="C422" t="s">
         <v>28</v>
@@ -38005,76 +38005,76 @@
         <v>44975.54166666666</v>
       </c>
       <c r="F422" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G422" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H422">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I422">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J422" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K422">
-        <v>2.2</v>
+        <v>4.75</v>
       </c>
       <c r="L422">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M422">
-        <v>3.1</v>
+        <v>1.727</v>
       </c>
       <c r="N422">
-        <v>2.55</v>
+        <v>5.75</v>
       </c>
       <c r="O422">
-        <v>3.3</v>
+        <v>4.2</v>
       </c>
       <c r="P422">
+        <v>1.6</v>
+      </c>
+      <c r="Q422">
+        <v>1</v>
+      </c>
+      <c r="R422">
+        <v>1.825</v>
+      </c>
+      <c r="S422">
+        <v>2.025</v>
+      </c>
+      <c r="T422">
         <v>2.75</v>
       </c>
-      <c r="Q422">
-        <v>0</v>
-      </c>
-      <c r="R422">
-        <v>1.85</v>
-      </c>
-      <c r="S422">
-        <v>2</v>
-      </c>
-      <c r="T422">
-        <v>2.5</v>
-      </c>
       <c r="U422">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V422">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W422">
         <v>-1</v>
       </c>
       <c r="X422">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y422">
-        <v>1.75</v>
+        <v>-1</v>
       </c>
       <c r="Z422">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA422">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB422">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AC422">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="423" spans="1:29">
@@ -38082,7 +38082,7 @@
         <v>421</v>
       </c>
       <c r="B423">
-        <v>5205973</v>
+        <v>5205971</v>
       </c>
       <c r="C423" t="s">
         <v>28</v>
@@ -38094,76 +38094,76 @@
         <v>44975.54166666666</v>
       </c>
       <c r="F423" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="G423" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H423">
+        <v>0</v>
+      </c>
+      <c r="I423">
+        <v>3</v>
+      </c>
+      <c r="J423" t="s">
+        <v>46</v>
+      </c>
+      <c r="K423">
+        <v>2.2</v>
+      </c>
+      <c r="L423">
+        <v>3.5</v>
+      </c>
+      <c r="M423">
+        <v>3.1</v>
+      </c>
+      <c r="N423">
+        <v>2.55</v>
+      </c>
+      <c r="O423">
+        <v>3.3</v>
+      </c>
+      <c r="P423">
+        <v>2.75</v>
+      </c>
+      <c r="Q423">
+        <v>0</v>
+      </c>
+      <c r="R423">
+        <v>1.85</v>
+      </c>
+      <c r="S423">
+        <v>2</v>
+      </c>
+      <c r="T423">
+        <v>2.5</v>
+      </c>
+      <c r="U423">
+        <v>1.875</v>
+      </c>
+      <c r="V423">
+        <v>1.975</v>
+      </c>
+      <c r="W423">
+        <v>-1</v>
+      </c>
+      <c r="X423">
+        <v>-1</v>
+      </c>
+      <c r="Y423">
+        <v>1.75</v>
+      </c>
+      <c r="Z423">
+        <v>-1</v>
+      </c>
+      <c r="AA423">
         <v>1</v>
       </c>
-      <c r="I423">
-        <v>1</v>
-      </c>
-      <c r="J423" t="s">
-        <v>44</v>
-      </c>
-      <c r="K423">
-        <v>4.75</v>
-      </c>
-      <c r="L423">
-        <v>3.6</v>
-      </c>
-      <c r="M423">
-        <v>1.727</v>
-      </c>
-      <c r="N423">
-        <v>5.75</v>
-      </c>
-      <c r="O423">
-        <v>4.2</v>
-      </c>
-      <c r="P423">
-        <v>1.6</v>
-      </c>
-      <c r="Q423">
-        <v>1</v>
-      </c>
-      <c r="R423">
-        <v>1.825</v>
-      </c>
-      <c r="S423">
-        <v>2.025</v>
-      </c>
-      <c r="T423">
-        <v>2.75</v>
-      </c>
-      <c r="U423">
-        <v>1.925</v>
-      </c>
-      <c r="V423">
-        <v>1.925</v>
-      </c>
-      <c r="W423">
-        <v>-1</v>
-      </c>
-      <c r="X423">
-        <v>3.2</v>
-      </c>
-      <c r="Y423">
-        <v>-1</v>
-      </c>
-      <c r="Z423">
-        <v>0.825</v>
-      </c>
-      <c r="AA423">
-        <v>-1</v>
-      </c>
       <c r="AB423">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AC423">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="424" spans="1:29">
@@ -38171,7 +38171,7 @@
         <v>422</v>
       </c>
       <c r="B424">
-        <v>5207167</v>
+        <v>5205975</v>
       </c>
       <c r="C424" t="s">
         <v>28</v>
@@ -38183,76 +38183,76 @@
         <v>44976.4375</v>
       </c>
       <c r="F424" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G424" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H424">
         <v>1</v>
       </c>
       <c r="I424">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J424" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K424">
-        <v>3.8</v>
+        <v>7</v>
       </c>
       <c r="L424">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="M424">
-        <v>1.95</v>
+        <v>1.4</v>
       </c>
       <c r="N424">
-        <v>4.2</v>
+        <v>6</v>
       </c>
       <c r="O424">
-        <v>3.6</v>
+        <v>4.75</v>
       </c>
       <c r="P424">
-        <v>1.85</v>
+        <v>1.5</v>
       </c>
       <c r="Q424">
+        <v>1.25</v>
+      </c>
+      <c r="R424">
+        <v>1.8</v>
+      </c>
+      <c r="S424">
+        <v>2.05</v>
+      </c>
+      <c r="T424">
+        <v>3</v>
+      </c>
+      <c r="U424">
+        <v>1.975</v>
+      </c>
+      <c r="V424">
+        <v>1.875</v>
+      </c>
+      <c r="W424">
+        <v>-1</v>
+      </c>
+      <c r="X424">
+        <v>-1</v>
+      </c>
+      <c r="Y424">
         <v>0.5</v>
       </c>
-      <c r="R424">
-        <v>1.975</v>
-      </c>
-      <c r="S424">
-        <v>1.875</v>
-      </c>
-      <c r="T424">
-        <v>2.5</v>
-      </c>
-      <c r="U424">
-        <v>1.825</v>
-      </c>
-      <c r="V424">
-        <v>2.025</v>
-      </c>
-      <c r="W424">
-        <v>3.2</v>
-      </c>
-      <c r="X424">
-        <v>-1</v>
-      </c>
-      <c r="Y424">
-        <v>-1</v>
-      </c>
       <c r="Z424">
+        <v>-1</v>
+      </c>
+      <c r="AA424">
+        <v>1.05</v>
+      </c>
+      <c r="AB424">
         <v>0.9750000000000001</v>
       </c>
-      <c r="AA424">
-        <v>-1</v>
-      </c>
-      <c r="AB424">
-        <v>-1</v>
-      </c>
       <c r="AC424">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="425" spans="1:29">
@@ -38260,7 +38260,7 @@
         <v>423</v>
       </c>
       <c r="B425">
-        <v>5205975</v>
+        <v>5207167</v>
       </c>
       <c r="C425" t="s">
         <v>28</v>
@@ -38272,76 +38272,76 @@
         <v>44976.4375</v>
       </c>
       <c r="F425" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G425" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H425">
         <v>1</v>
       </c>
       <c r="I425">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J425" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K425">
-        <v>7</v>
+        <v>3.8</v>
       </c>
       <c r="L425">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="M425">
-        <v>1.4</v>
+        <v>1.95</v>
       </c>
       <c r="N425">
-        <v>6</v>
+        <v>4.2</v>
       </c>
       <c r="O425">
-        <v>4.75</v>
+        <v>3.6</v>
       </c>
       <c r="P425">
-        <v>1.5</v>
+        <v>1.85</v>
       </c>
       <c r="Q425">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="R425">
-        <v>1.8</v>
+        <v>1.975</v>
       </c>
       <c r="S425">
-        <v>2.05</v>
+        <v>1.875</v>
       </c>
       <c r="T425">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U425">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V425">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W425">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="X425">
         <v>-1</v>
       </c>
       <c r="Y425">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z425">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA425">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB425">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC425">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="426" spans="1:29">
@@ -39862,7 +39862,7 @@
         <v>441</v>
       </c>
       <c r="B443">
-        <v>5207164</v>
+        <v>5205988</v>
       </c>
       <c r="C443" t="s">
         <v>28</v>
@@ -39874,76 +39874,76 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F443" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="G443" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H443">
+        <v>1</v>
+      </c>
+      <c r="I443">
         <v>0</v>
       </c>
-      <c r="I443">
-        <v>1</v>
-      </c>
       <c r="J443" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K443">
-        <v>1.75</v>
+        <v>1.909</v>
       </c>
       <c r="L443">
         <v>3.6</v>
       </c>
       <c r="M443">
-        <v>4.5</v>
+        <v>3.8</v>
       </c>
       <c r="N443">
-        <v>1.7</v>
+        <v>2.15</v>
       </c>
       <c r="O443">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="P443">
-        <v>5.25</v>
+        <v>3.3</v>
       </c>
       <c r="Q443">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R443">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="S443">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="T443">
         <v>2.75</v>
       </c>
       <c r="U443">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V443">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W443">
-        <v>-1</v>
+        <v>1.15</v>
       </c>
       <c r="X443">
         <v>-1</v>
       </c>
       <c r="Y443">
-        <v>4.25</v>
+        <v>-1</v>
       </c>
       <c r="Z443">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA443">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB443">
         <v>-1</v>
       </c>
       <c r="AC443">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="444" spans="1:29">
@@ -39951,7 +39951,7 @@
         <v>442</v>
       </c>
       <c r="B444">
-        <v>5205988</v>
+        <v>5207164</v>
       </c>
       <c r="C444" t="s">
         <v>28</v>
@@ -39963,76 +39963,76 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F444" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="G444" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H444">
+        <v>0</v>
+      </c>
+      <c r="I444">
         <v>1</v>
       </c>
-      <c r="I444">
-        <v>0</v>
-      </c>
       <c r="J444" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K444">
-        <v>1.909</v>
+        <v>1.75</v>
       </c>
       <c r="L444">
         <v>3.6</v>
       </c>
       <c r="M444">
+        <v>4.5</v>
+      </c>
+      <c r="N444">
+        <v>1.7</v>
+      </c>
+      <c r="O444">
         <v>3.8</v>
       </c>
-      <c r="N444">
-        <v>2.15</v>
-      </c>
-      <c r="O444">
-        <v>3.4</v>
-      </c>
       <c r="P444">
-        <v>3.3</v>
+        <v>5.25</v>
       </c>
       <c r="Q444">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R444">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="S444">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="T444">
         <v>2.75</v>
       </c>
       <c r="U444">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V444">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W444">
-        <v>1.15</v>
+        <v>-1</v>
       </c>
       <c r="X444">
         <v>-1</v>
       </c>
       <c r="Y444">
-        <v>-1</v>
+        <v>4.25</v>
       </c>
       <c r="Z444">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA444">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB444">
         <v>-1</v>
       </c>
       <c r="AC444">
-        <v>0.8500000000000001</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="445" spans="1:29">
@@ -46092,7 +46092,7 @@
         <v>511</v>
       </c>
       <c r="B513">
-        <v>6847026</v>
+        <v>6847027</v>
       </c>
       <c r="C513" t="s">
         <v>28</v>
@@ -46104,73 +46104,73 @@
         <v>45136.5</v>
       </c>
       <c r="F513" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G513" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H513">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I513">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J513" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K513">
         <v>2.1</v>
       </c>
       <c r="L513">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M513">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="N513">
-        <v>1.833</v>
+        <v>2.3</v>
       </c>
       <c r="O513">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P513">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="Q513">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R513">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S513">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="T513">
         <v>2.75</v>
       </c>
       <c r="U513">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V513">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W513">
         <v>-1</v>
       </c>
       <c r="X513">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y513">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z513">
         <v>-1</v>
       </c>
       <c r="AA513">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB513">
-        <v>0.925</v>
+        <v>0.825</v>
       </c>
       <c r="AC513">
         <v>-1</v>
@@ -46181,7 +46181,7 @@
         <v>512</v>
       </c>
       <c r="B514">
-        <v>6847027</v>
+        <v>6847026</v>
       </c>
       <c r="C514" t="s">
         <v>28</v>
@@ -46193,73 +46193,73 @@
         <v>45136.5</v>
       </c>
       <c r="F514" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G514" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H514">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I514">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J514" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K514">
         <v>2.1</v>
       </c>
       <c r="L514">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="M514">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="N514">
-        <v>2.3</v>
+        <v>1.833</v>
       </c>
       <c r="O514">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P514">
-        <v>2.8</v>
+        <v>4.2</v>
       </c>
       <c r="Q514">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R514">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="S514">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="T514">
         <v>2.75</v>
       </c>
       <c r="U514">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V514">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W514">
         <v>-1</v>
       </c>
       <c r="X514">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y514">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z514">
         <v>-1</v>
       </c>
       <c r="AA514">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB514">
-        <v>0.825</v>
+        <v>0.925</v>
       </c>
       <c r="AC514">
         <v>-1</v>
@@ -47783,7 +47783,7 @@
         <v>530</v>
       </c>
       <c r="B532">
-        <v>6846461</v>
+        <v>6847040</v>
       </c>
       <c r="C532" t="s">
         <v>28</v>
@@ -47795,76 +47795,76 @@
         <v>45158.5</v>
       </c>
       <c r="F532" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G532" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H532">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I532">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J532" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K532">
-        <v>9.5</v>
+        <v>1.85</v>
       </c>
       <c r="L532">
-        <v>4.8</v>
+        <v>3.6</v>
       </c>
       <c r="M532">
-        <v>1.3</v>
+        <v>3.8</v>
       </c>
       <c r="N532">
-        <v>5.75</v>
+        <v>2</v>
       </c>
       <c r="O532">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="P532">
-        <v>1.55</v>
+        <v>3.6</v>
       </c>
       <c r="Q532">
-        <v>1</v>
+        <v>-0.5</v>
       </c>
       <c r="R532">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="S532">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="T532">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U532">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="V532">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="W532">
         <v>-1</v>
       </c>
       <c r="X532">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y532">
-        <v>0.55</v>
+        <v>-1</v>
       </c>
       <c r="Z532">
         <v>-1</v>
       </c>
       <c r="AA532">
-        <v>0.95</v>
+        <v>0.825</v>
       </c>
       <c r="AB532">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC532">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="533" spans="1:29">
@@ -47872,7 +47872,7 @@
         <v>531</v>
       </c>
       <c r="B533">
-        <v>6851961</v>
+        <v>6846461</v>
       </c>
       <c r="C533" t="s">
         <v>28</v>
@@ -47884,13 +47884,13 @@
         <v>45158.5</v>
       </c>
       <c r="F533" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G533" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H533">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I533">
         <v>5</v>
@@ -47899,40 +47899,40 @@
         <v>46</v>
       </c>
       <c r="K533">
-        <v>4.333</v>
+        <v>9.5</v>
       </c>
       <c r="L533">
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="M533">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="N533">
-        <v>3.5</v>
+        <v>5.75</v>
       </c>
       <c r="O533">
-        <v>3.75</v>
+        <v>4.2</v>
       </c>
       <c r="P533">
+        <v>1.55</v>
+      </c>
+      <c r="Q533">
+        <v>1</v>
+      </c>
+      <c r="R533">
+        <v>1.9</v>
+      </c>
+      <c r="S533">
         <v>1.95</v>
       </c>
-      <c r="Q533">
-        <v>0.5</v>
-      </c>
-      <c r="R533">
+      <c r="T533">
+        <v>3</v>
+      </c>
+      <c r="U533">
         <v>1.85</v>
       </c>
-      <c r="S533">
-        <v>2</v>
-      </c>
-      <c r="T533">
-        <v>2.75</v>
-      </c>
-      <c r="U533">
-        <v>1.925</v>
-      </c>
       <c r="V533">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="W533">
         <v>-1</v>
@@ -47941,16 +47941,16 @@
         <v>-1</v>
       </c>
       <c r="Y533">
+        <v>0.55</v>
+      </c>
+      <c r="Z533">
+        <v>-1</v>
+      </c>
+      <c r="AA533">
         <v>0.95</v>
       </c>
-      <c r="Z533">
-        <v>-1</v>
-      </c>
-      <c r="AA533">
-        <v>1</v>
-      </c>
       <c r="AB533">
-        <v>0.925</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC533">
         <v>-1</v>
@@ -47961,7 +47961,7 @@
         <v>532</v>
       </c>
       <c r="B534">
-        <v>6847040</v>
+        <v>6851961</v>
       </c>
       <c r="C534" t="s">
         <v>28</v>
@@ -47973,76 +47973,76 @@
         <v>45158.5</v>
       </c>
       <c r="F534" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G534" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H534">
         <v>0</v>
       </c>
       <c r="I534">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J534" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K534">
+        <v>4.333</v>
+      </c>
+      <c r="L534">
+        <v>3.8</v>
+      </c>
+      <c r="M534">
+        <v>1.7</v>
+      </c>
+      <c r="N534">
+        <v>3.5</v>
+      </c>
+      <c r="O534">
+        <v>3.75</v>
+      </c>
+      <c r="P534">
+        <v>1.95</v>
+      </c>
+      <c r="Q534">
+        <v>0.5</v>
+      </c>
+      <c r="R534">
         <v>1.85</v>
       </c>
-      <c r="L534">
-        <v>3.6</v>
-      </c>
-      <c r="M534">
-        <v>3.8</v>
-      </c>
-      <c r="N534">
-        <v>2</v>
-      </c>
-      <c r="O534">
-        <v>3.4</v>
-      </c>
-      <c r="P534">
-        <v>3.6</v>
-      </c>
-      <c r="Q534">
-        <v>-0.5</v>
-      </c>
-      <c r="R534">
-        <v>2.025</v>
-      </c>
       <c r="S534">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="T534">
         <v>2.75</v>
       </c>
       <c r="U534">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V534">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W534">
         <v>-1</v>
       </c>
       <c r="X534">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y534">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z534">
         <v>-1</v>
       </c>
       <c r="AA534">
-        <v>0.825</v>
+        <v>1</v>
       </c>
       <c r="AB534">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC534">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="535" spans="1:29">
@@ -49919,7 +49919,7 @@
         <v>554</v>
       </c>
       <c r="B556">
-        <v>6847053</v>
+        <v>6847056</v>
       </c>
       <c r="C556" t="s">
         <v>28</v>
@@ -49931,76 +49931,76 @@
         <v>45193.39583333334</v>
       </c>
       <c r="F556" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G556" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H556">
+        <v>2</v>
+      </c>
+      <c r="I556">
+        <v>1</v>
+      </c>
+      <c r="J556" t="s">
+        <v>45</v>
+      </c>
+      <c r="K556">
+        <v>3.75</v>
+      </c>
+      <c r="L556">
+        <v>3.5</v>
+      </c>
+      <c r="M556">
+        <v>1.95</v>
+      </c>
+      <c r="N556">
+        <v>3</v>
+      </c>
+      <c r="O556">
+        <v>3.3</v>
+      </c>
+      <c r="P556">
+        <v>2.4</v>
+      </c>
+      <c r="Q556">
         <v>0</v>
       </c>
-      <c r="I556">
-        <v>0</v>
-      </c>
-      <c r="J556" t="s">
-        <v>44</v>
-      </c>
-      <c r="K556">
-        <v>1.571</v>
-      </c>
-      <c r="L556">
-        <v>4.333</v>
-      </c>
-      <c r="M556">
-        <v>5</v>
-      </c>
-      <c r="N556">
-        <v>1.727</v>
-      </c>
-      <c r="O556">
-        <v>4</v>
-      </c>
-      <c r="P556">
-        <v>4.5</v>
-      </c>
-      <c r="Q556">
-        <v>-0.75</v>
-      </c>
       <c r="R556">
-        <v>1.95</v>
+        <v>2.1</v>
       </c>
       <c r="S556">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="T556">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U556">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V556">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="W556">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="X556">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y556">
         <v>-1</v>
       </c>
       <c r="Z556">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="AA556">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB556">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC556">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="557" spans="1:29">
@@ -50008,7 +50008,7 @@
         <v>555</v>
       </c>
       <c r="B557">
-        <v>6847056</v>
+        <v>6847053</v>
       </c>
       <c r="C557" t="s">
         <v>28</v>
@@ -50020,76 +50020,76 @@
         <v>45193.39583333334</v>
       </c>
       <c r="F557" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G557" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H557">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I557">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J557" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K557">
-        <v>3.75</v>
+        <v>1.571</v>
       </c>
       <c r="L557">
-        <v>3.5</v>
+        <v>4.333</v>
       </c>
       <c r="M557">
+        <v>5</v>
+      </c>
+      <c r="N557">
+        <v>1.727</v>
+      </c>
+      <c r="O557">
+        <v>4</v>
+      </c>
+      <c r="P557">
+        <v>4.5</v>
+      </c>
+      <c r="Q557">
+        <v>-0.75</v>
+      </c>
+      <c r="R557">
         <v>1.95</v>
       </c>
-      <c r="N557">
+      <c r="S557">
+        <v>1.9</v>
+      </c>
+      <c r="T557">
+        <v>2.75</v>
+      </c>
+      <c r="U557">
+        <v>1.8</v>
+      </c>
+      <c r="V557">
+        <v>2.05</v>
+      </c>
+      <c r="W557">
+        <v>-1</v>
+      </c>
+      <c r="X557">
         <v>3</v>
       </c>
-      <c r="O557">
-        <v>3.3</v>
-      </c>
-      <c r="P557">
-        <v>2.4</v>
-      </c>
-      <c r="Q557">
-        <v>0</v>
-      </c>
-      <c r="R557">
-        <v>2.1</v>
-      </c>
-      <c r="S557">
-        <v>1.775</v>
-      </c>
-      <c r="T557">
-        <v>2.5</v>
-      </c>
-      <c r="U557">
-        <v>1.925</v>
-      </c>
-      <c r="V557">
-        <v>1.925</v>
-      </c>
-      <c r="W557">
-        <v>2</v>
-      </c>
-      <c r="X557">
-        <v>-1</v>
-      </c>
       <c r="Y557">
         <v>-1</v>
       </c>
       <c r="Z557">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="AA557">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB557">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC557">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="558" spans="1:29">
@@ -50453,7 +50453,7 @@
         <v>560</v>
       </c>
       <c r="B562">
-        <v>6847060</v>
+        <v>6847061</v>
       </c>
       <c r="C562" t="s">
         <v>28</v>
@@ -50465,61 +50465,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F562" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G562" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H562">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I562">
         <v>0</v>
       </c>
       <c r="J562" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K562">
-        <v>1.25</v>
+        <v>1.909</v>
       </c>
       <c r="L562">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M562">
-        <v>10</v>
+        <v>3.9</v>
       </c>
       <c r="N562">
-        <v>1.285</v>
+        <v>2</v>
       </c>
       <c r="O562">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="P562">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="Q562">
-        <v>-1.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R562">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="S562">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="T562">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U562">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V562">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W562">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X562">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y562">
         <v>-1</v>
@@ -50528,13 +50528,13 @@
         <v>-1</v>
       </c>
       <c r="AA562">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AB562">
         <v>-1</v>
       </c>
       <c r="AC562">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="563" spans="1:29">
@@ -50542,7 +50542,7 @@
         <v>561</v>
       </c>
       <c r="B563">
-        <v>6847061</v>
+        <v>6847060</v>
       </c>
       <c r="C563" t="s">
         <v>28</v>
@@ -50554,61 +50554,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F563" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G563" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H563">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I563">
         <v>0</v>
       </c>
       <c r="J563" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K563">
-        <v>1.909</v>
+        <v>1.25</v>
       </c>
       <c r="L563">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M563">
-        <v>3.9</v>
+        <v>10</v>
       </c>
       <c r="N563">
-        <v>2</v>
+        <v>1.285</v>
       </c>
       <c r="O563">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="P563">
-        <v>3.6</v>
+        <v>9</v>
       </c>
       <c r="Q563">
-        <v>-0.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R563">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="S563">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="T563">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U563">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V563">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W563">
-        <v>-1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="X563">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y563">
         <v>-1</v>
@@ -50617,13 +50617,13 @@
         <v>-1</v>
       </c>
       <c r="AA563">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AB563">
         <v>-1</v>
       </c>
       <c r="AC563">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="564" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-29 às 18-52
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -31229,7 +31229,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>5205909</v>
+        <v>5205910</v>
       </c>
       <c r="C346" t="s">
         <v>28</v>
@@ -31241,10 +31241,10 @@
         <v>44794.5</v>
       </c>
       <c r="F346" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G346" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H346">
         <v>1</v>
@@ -31256,40 +31256,40 @@
         <v>46</v>
       </c>
       <c r="K346">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="L346">
         <v>3.25</v>
       </c>
       <c r="M346">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="N346">
-        <v>2.7</v>
+        <v>2.375</v>
       </c>
       <c r="O346">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P346">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="Q346">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R346">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S346">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T346">
         <v>2.75</v>
       </c>
       <c r="U346">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V346">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W346">
         <v>-1</v>
@@ -31298,16 +31298,16 @@
         <v>-1</v>
       </c>
       <c r="Y346">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="Z346">
         <v>-1</v>
       </c>
       <c r="AA346">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB346">
-        <v>0.4375</v>
+        <v>0.4625</v>
       </c>
       <c r="AC346">
         <v>-0.5</v>
@@ -31318,7 +31318,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>5205910</v>
+        <v>5205909</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31330,10 +31330,10 @@
         <v>44794.5</v>
       </c>
       <c r="F347" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G347" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H347">
         <v>1</v>
@@ -31345,40 +31345,40 @@
         <v>46</v>
       </c>
       <c r="K347">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="L347">
         <v>3.25</v>
       </c>
       <c r="M347">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="N347">
-        <v>2.375</v>
+        <v>2.7</v>
       </c>
       <c r="O347">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P347">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="Q347">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R347">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="S347">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T347">
         <v>2.75</v>
       </c>
       <c r="U347">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V347">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W347">
         <v>-1</v>
@@ -31387,16 +31387,16 @@
         <v>-1</v>
       </c>
       <c r="Y347">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="Z347">
         <v>-1</v>
       </c>
       <c r="AA347">
-        <v>0.8500000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB347">
-        <v>0.4625</v>
+        <v>0.4375</v>
       </c>
       <c r="AC347">
         <v>-0.5</v>
@@ -31674,7 +31674,7 @@
         <v>349</v>
       </c>
       <c r="B351">
-        <v>5205914</v>
+        <v>5205913</v>
       </c>
       <c r="C351" t="s">
         <v>28</v>
@@ -31686,40 +31686,40 @@
         <v>44801.5</v>
       </c>
       <c r="F351" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G351" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H351">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I351">
         <v>3</v>
       </c>
       <c r="J351" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K351">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="L351">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="M351">
-        <v>2.3</v>
+        <v>2.375</v>
       </c>
       <c r="N351">
-        <v>2.75</v>
+        <v>2.375</v>
       </c>
       <c r="O351">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="P351">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
       <c r="Q351">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R351">
         <v>2.025</v>
@@ -31728,31 +31728,31 @@
         <v>1.825</v>
       </c>
       <c r="T351">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U351">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V351">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W351">
         <v>-1</v>
       </c>
       <c r="X351">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y351">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z351">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA351">
-        <v>-0</v>
+        <v>0.825</v>
       </c>
       <c r="AB351">
-        <v>0.9750000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AC351">
         <v>-1</v>
@@ -31763,7 +31763,7 @@
         <v>350</v>
       </c>
       <c r="B352">
-        <v>5205915</v>
+        <v>5205914</v>
       </c>
       <c r="C352" t="s">
         <v>28</v>
@@ -31775,73 +31775,73 @@
         <v>44801.5</v>
       </c>
       <c r="F352" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G352" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H352">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I352">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J352" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K352">
-        <v>2.55</v>
+        <v>3</v>
       </c>
       <c r="L352">
         <v>3.4</v>
       </c>
       <c r="M352">
-        <v>2.625</v>
+        <v>2.3</v>
       </c>
       <c r="N352">
-        <v>2.875</v>
+        <v>2.75</v>
       </c>
       <c r="O352">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="P352">
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="Q352">
         <v>0</v>
       </c>
       <c r="R352">
-        <v>2.05</v>
+        <v>2.025</v>
       </c>
       <c r="S352">
-        <v>1.75</v>
+        <v>1.825</v>
       </c>
       <c r="T352">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U352">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V352">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W352">
         <v>-1</v>
       </c>
       <c r="X352">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y352">
-        <v>1.4</v>
+        <v>-1</v>
       </c>
       <c r="Z352">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA352">
-        <v>0.75</v>
+        <v>-0</v>
       </c>
       <c r="AB352">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC352">
         <v>-1</v>
@@ -31852,7 +31852,7 @@
         <v>351</v>
       </c>
       <c r="B353">
-        <v>5205913</v>
+        <v>5205915</v>
       </c>
       <c r="C353" t="s">
         <v>28</v>
@@ -31864,56 +31864,56 @@
         <v>44801.5</v>
       </c>
       <c r="F353" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G353" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H353">
         <v>1</v>
       </c>
       <c r="I353">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J353" t="s">
         <v>46</v>
       </c>
       <c r="K353">
-        <v>2.8</v>
+        <v>2.55</v>
       </c>
       <c r="L353">
+        <v>3.4</v>
+      </c>
+      <c r="M353">
+        <v>2.625</v>
+      </c>
+      <c r="N353">
+        <v>2.875</v>
+      </c>
+      <c r="O353">
         <v>3.5</v>
       </c>
-      <c r="M353">
-        <v>2.375</v>
-      </c>
-      <c r="N353">
-        <v>2.375</v>
-      </c>
-      <c r="O353">
-        <v>3.75</v>
-      </c>
       <c r="P353">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="Q353">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R353">
+        <v>2.05</v>
+      </c>
+      <c r="S353">
+        <v>1.75</v>
+      </c>
+      <c r="T353">
+        <v>2.5</v>
+      </c>
+      <c r="U353">
+        <v>1.825</v>
+      </c>
+      <c r="V353">
         <v>2.025</v>
       </c>
-      <c r="S353">
-        <v>1.825</v>
-      </c>
-      <c r="T353">
-        <v>3</v>
-      </c>
-      <c r="U353">
-        <v>1.925</v>
-      </c>
-      <c r="V353">
-        <v>1.925</v>
-      </c>
       <c r="W353">
         <v>-1</v>
       </c>
@@ -31921,16 +31921,16 @@
         <v>-1</v>
       </c>
       <c r="Y353">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="Z353">
         <v>-1</v>
       </c>
       <c r="AA353">
+        <v>0.75</v>
+      </c>
+      <c r="AB353">
         <v>0.825</v>
-      </c>
-      <c r="AB353">
-        <v>0.925</v>
       </c>
       <c r="AC353">
         <v>-1</v>
@@ -33009,7 +33009,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>5205930</v>
+        <v>5205928</v>
       </c>
       <c r="C366" t="s">
         <v>28</v>
@@ -33021,73 +33021,73 @@
         <v>44821.5</v>
       </c>
       <c r="F366" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G366" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H366">
+        <v>3</v>
+      </c>
+      <c r="I366">
         <v>1</v>
       </c>
-      <c r="I366">
+      <c r="J366" t="s">
+        <v>45</v>
+      </c>
+      <c r="K366">
+        <v>1.666</v>
+      </c>
+      <c r="L366">
         <v>4</v>
       </c>
-      <c r="J366" t="s">
-        <v>46</v>
-      </c>
-      <c r="K366">
+      <c r="M366">
+        <v>4.333</v>
+      </c>
+      <c r="N366">
+        <v>1.727</v>
+      </c>
+      <c r="O366">
+        <v>4.333</v>
+      </c>
+      <c r="P366">
+        <v>4</v>
+      </c>
+      <c r="Q366">
+        <v>-0.75</v>
+      </c>
+      <c r="R366">
+        <v>1.95</v>
+      </c>
+      <c r="S366">
+        <v>1.9</v>
+      </c>
+      <c r="T366">
         <v>3</v>
       </c>
-      <c r="L366">
-        <v>3.5</v>
-      </c>
-      <c r="M366">
-        <v>2.2</v>
-      </c>
-      <c r="N366">
-        <v>2.8</v>
-      </c>
-      <c r="O366">
-        <v>3.5</v>
-      </c>
-      <c r="P366">
-        <v>2.375</v>
-      </c>
-      <c r="Q366">
-        <v>0.25</v>
-      </c>
-      <c r="R366">
-        <v>1.8</v>
-      </c>
-      <c r="S366">
-        <v>2.05</v>
-      </c>
-      <c r="T366">
-        <v>2.75</v>
-      </c>
       <c r="U366">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V366">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W366">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="X366">
         <v>-1</v>
       </c>
       <c r="Y366">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Z366">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA366">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AB366">
-        <v>0.9750000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AC366">
         <v>-1</v>
@@ -33098,7 +33098,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>5205928</v>
+        <v>5205927</v>
       </c>
       <c r="C367" t="s">
         <v>28</v>
@@ -33110,73 +33110,73 @@
         <v>44821.5</v>
       </c>
       <c r="F367" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G367" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H367">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I367">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J367" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K367">
-        <v>1.666</v>
+        <v>1.363</v>
       </c>
       <c r="L367">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M367">
-        <v>4.333</v>
+        <v>8</v>
       </c>
       <c r="N367">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="O367">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="P367">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q367">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="R367">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="S367">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T367">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U367">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V367">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W367">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X367">
         <v>-1</v>
       </c>
       <c r="Y367">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Z367">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA367">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB367">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
       <c r="AC367">
         <v>-1</v>
@@ -33187,7 +33187,7 @@
         <v>366</v>
       </c>
       <c r="B368">
-        <v>5205927</v>
+        <v>5205930</v>
       </c>
       <c r="C368" t="s">
         <v>28</v>
@@ -33199,10 +33199,10 @@
         <v>44821.5</v>
       </c>
       <c r="F368" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G368" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H368">
         <v>1</v>
@@ -33214,40 +33214,40 @@
         <v>46</v>
       </c>
       <c r="K368">
-        <v>1.363</v>
+        <v>3</v>
       </c>
       <c r="L368">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="M368">
-        <v>8</v>
+        <v>2.2</v>
       </c>
       <c r="N368">
-        <v>1.5</v>
+        <v>2.8</v>
       </c>
       <c r="O368">
-        <v>4.75</v>
+        <v>3.5</v>
       </c>
       <c r="P368">
-        <v>6</v>
+        <v>2.375</v>
       </c>
       <c r="Q368">
-        <v>-1.25</v>
+        <v>0.25</v>
       </c>
       <c r="R368">
+        <v>1.8</v>
+      </c>
+      <c r="S368">
         <v>2.05</v>
       </c>
-      <c r="S368">
-        <v>1.8</v>
-      </c>
       <c r="T368">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U368">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V368">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W368">
         <v>-1</v>
@@ -33256,16 +33256,16 @@
         <v>-1</v>
       </c>
       <c r="Y368">
-        <v>5</v>
+        <v>1.375</v>
       </c>
       <c r="Z368">
         <v>-1</v>
       </c>
       <c r="AA368">
-        <v>0.8</v>
+        <v>1.05</v>
       </c>
       <c r="AB368">
-        <v>1.025</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC368">
         <v>-1</v>
@@ -34077,7 +34077,7 @@
         <v>376</v>
       </c>
       <c r="B378">
-        <v>5207174</v>
+        <v>5205936</v>
       </c>
       <c r="C378" t="s">
         <v>28</v>
@@ -34089,76 +34089,76 @@
         <v>44842.5</v>
       </c>
       <c r="F378" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G378" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H378">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I378">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J378" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K378">
-        <v>1.85</v>
+        <v>1.45</v>
       </c>
       <c r="L378">
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="M378">
-        <v>3.6</v>
+        <v>5.75</v>
       </c>
       <c r="N378">
-        <v>1.7</v>
+        <v>1.333</v>
       </c>
       <c r="O378">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="P378">
-        <v>4.333</v>
+        <v>8</v>
       </c>
       <c r="Q378">
-        <v>-0.75</v>
+        <v>-1.5</v>
       </c>
       <c r="R378">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="S378">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="T378">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U378">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V378">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="W378">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="X378">
         <v>-1</v>
       </c>
       <c r="Y378">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="Z378">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AA378">
+        <v>0.925</v>
+      </c>
+      <c r="AB378">
         <v>-0.5</v>
       </c>
-      <c r="AB378">
-        <v>0</v>
-      </c>
       <c r="AC378">
-        <v>-0</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="379" spans="1:29">
@@ -34255,7 +34255,7 @@
         <v>378</v>
       </c>
       <c r="B380">
-        <v>5205936</v>
+        <v>5207174</v>
       </c>
       <c r="C380" t="s">
         <v>28</v>
@@ -34267,76 +34267,76 @@
         <v>44842.5</v>
       </c>
       <c r="F380" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G380" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H380">
+        <v>2</v>
+      </c>
+      <c r="I380">
+        <v>1</v>
+      </c>
+      <c r="J380" t="s">
+        <v>45</v>
+      </c>
+      <c r="K380">
+        <v>1.85</v>
+      </c>
+      <c r="L380">
+        <v>3.8</v>
+      </c>
+      <c r="M380">
+        <v>3.6</v>
+      </c>
+      <c r="N380">
+        <v>1.7</v>
+      </c>
+      <c r="O380">
+        <v>4</v>
+      </c>
+      <c r="P380">
+        <v>4.333</v>
+      </c>
+      <c r="Q380">
+        <v>-0.75</v>
+      </c>
+      <c r="R380">
+        <v>1.875</v>
+      </c>
+      <c r="S380">
+        <v>1.975</v>
+      </c>
+      <c r="T380">
+        <v>3</v>
+      </c>
+      <c r="U380">
+        <v>1.875</v>
+      </c>
+      <c r="V380">
+        <v>1.975</v>
+      </c>
+      <c r="W380">
+        <v>0.7</v>
+      </c>
+      <c r="X380">
+        <v>-1</v>
+      </c>
+      <c r="Y380">
+        <v>-1</v>
+      </c>
+      <c r="Z380">
+        <v>0.4375</v>
+      </c>
+      <c r="AA380">
+        <v>-0.5</v>
+      </c>
+      <c r="AB380">
         <v>0</v>
       </c>
-      <c r="I380">
-        <v>3</v>
-      </c>
-      <c r="J380" t="s">
-        <v>46</v>
-      </c>
-      <c r="K380">
-        <v>1.45</v>
-      </c>
-      <c r="L380">
-        <v>4.5</v>
-      </c>
-      <c r="M380">
-        <v>5.75</v>
-      </c>
-      <c r="N380">
-        <v>1.333</v>
-      </c>
-      <c r="O380">
-        <v>5.5</v>
-      </c>
-      <c r="P380">
-        <v>8</v>
-      </c>
-      <c r="Q380">
-        <v>-1.5</v>
-      </c>
-      <c r="R380">
-        <v>1.925</v>
-      </c>
-      <c r="S380">
-        <v>1.925</v>
-      </c>
-      <c r="T380">
-        <v>3.25</v>
-      </c>
-      <c r="U380">
-        <v>2.025</v>
-      </c>
-      <c r="V380">
-        <v>1.825</v>
-      </c>
-      <c r="W380">
-        <v>-1</v>
-      </c>
-      <c r="X380">
-        <v>-1</v>
-      </c>
-      <c r="Y380">
-        <v>7</v>
-      </c>
-      <c r="Z380">
-        <v>-1</v>
-      </c>
-      <c r="AA380">
-        <v>0.925</v>
-      </c>
-      <c r="AB380">
-        <v>-0.5</v>
-      </c>
       <c r="AC380">
-        <v>0.4125</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="381" spans="1:29">
@@ -35768,7 +35768,7 @@
         <v>395</v>
       </c>
       <c r="B397">
-        <v>5205951</v>
+        <v>5207171</v>
       </c>
       <c r="C397" t="s">
         <v>28</v>
@@ -35780,76 +35780,76 @@
         <v>44863.5</v>
       </c>
       <c r="F397" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G397" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H397">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I397">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J397" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K397">
-        <v>1.181</v>
+        <v>3.3</v>
       </c>
       <c r="L397">
-        <v>7</v>
+        <v>3.75</v>
       </c>
       <c r="M397">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="N397">
-        <v>1.222</v>
+        <v>4.75</v>
       </c>
       <c r="O397">
-        <v>7</v>
+        <v>4.2</v>
       </c>
       <c r="P397">
-        <v>11</v>
+        <v>1.65</v>
       </c>
       <c r="Q397">
-        <v>-2</v>
+        <v>0.75</v>
       </c>
       <c r="R397">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="S397">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T397">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U397">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="V397">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="W397">
-        <v>0.222</v>
+        <v>-1</v>
       </c>
       <c r="X397">
-        <v>-1</v>
+        <v>3.2</v>
       </c>
       <c r="Y397">
         <v>-1</v>
       </c>
       <c r="Z397">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA397">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB397">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC397">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="398" spans="1:29">
@@ -35857,7 +35857,7 @@
         <v>396</v>
       </c>
       <c r="B398">
-        <v>5207171</v>
+        <v>5205955</v>
       </c>
       <c r="C398" t="s">
         <v>28</v>
@@ -35869,73 +35869,73 @@
         <v>44863.5</v>
       </c>
       <c r="F398" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G398" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H398">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I398">
         <v>3</v>
       </c>
       <c r="J398" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K398">
-        <v>3.3</v>
+        <v>2</v>
       </c>
       <c r="L398">
+        <v>3.8</v>
+      </c>
+      <c r="M398">
+        <v>3.2</v>
+      </c>
+      <c r="N398">
+        <v>2</v>
+      </c>
+      <c r="O398">
         <v>3.75</v>
       </c>
-      <c r="M398">
-        <v>2</v>
-      </c>
-      <c r="N398">
-        <v>4.75</v>
-      </c>
-      <c r="O398">
-        <v>4.2</v>
-      </c>
       <c r="P398">
-        <v>1.65</v>
+        <v>3.4</v>
       </c>
       <c r="Q398">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R398">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S398">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T398">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U398">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V398">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W398">
         <v>-1</v>
       </c>
       <c r="X398">
-        <v>3.2</v>
+        <v>-1</v>
       </c>
       <c r="Y398">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Z398">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA398">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB398">
-        <v>0.825</v>
+        <v>1</v>
       </c>
       <c r="AC398">
         <v>-1</v>
@@ -35946,7 +35946,7 @@
         <v>397</v>
       </c>
       <c r="B399">
-        <v>5205955</v>
+        <v>5205951</v>
       </c>
       <c r="C399" t="s">
         <v>28</v>
@@ -35958,76 +35958,76 @@
         <v>44863.5</v>
       </c>
       <c r="F399" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G399" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H399">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I399">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J399" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K399">
-        <v>2</v>
+        <v>1.181</v>
       </c>
       <c r="L399">
-        <v>3.8</v>
+        <v>7</v>
       </c>
       <c r="M399">
-        <v>3.2</v>
+        <v>12</v>
       </c>
       <c r="N399">
-        <v>2</v>
+        <v>1.222</v>
       </c>
       <c r="O399">
-        <v>3.75</v>
+        <v>7</v>
       </c>
       <c r="P399">
-        <v>3.4</v>
+        <v>11</v>
       </c>
       <c r="Q399">
-        <v>-0.5</v>
+        <v>-2</v>
       </c>
       <c r="R399">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S399">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="T399">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="U399">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="V399">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="W399">
-        <v>-1</v>
+        <v>0.222</v>
       </c>
       <c r="X399">
         <v>-1</v>
       </c>
       <c r="Y399">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Z399">
         <v>-1</v>
       </c>
       <c r="AA399">
-        <v>0.825</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB399">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AC399">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="400" spans="1:29">
@@ -36302,7 +36302,7 @@
         <v>401</v>
       </c>
       <c r="B403">
-        <v>5205956</v>
+        <v>5207170</v>
       </c>
       <c r="C403" t="s">
         <v>28</v>
@@ -36314,76 +36314,76 @@
         <v>44870.54166666666</v>
       </c>
       <c r="F403" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G403" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H403">
         <v>1</v>
       </c>
       <c r="I403">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J403" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K403">
-        <v>5</v>
+        <v>2.375</v>
       </c>
       <c r="L403">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="M403">
-        <v>1.6</v>
+        <v>2.9</v>
       </c>
       <c r="N403">
-        <v>9</v>
+        <v>2.3</v>
       </c>
       <c r="O403">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="P403">
-        <v>1.333</v>
+        <v>3.1</v>
       </c>
       <c r="Q403">
-        <v>1.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R403">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="S403">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="T403">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U403">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V403">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W403">
         <v>-1</v>
       </c>
       <c r="X403">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y403">
-        <v>0.333</v>
+        <v>-1</v>
       </c>
       <c r="Z403">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AA403">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AB403">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC403">
-        <v>0.4625</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="404" spans="1:29">
@@ -36391,7 +36391,7 @@
         <v>402</v>
       </c>
       <c r="B404">
-        <v>5207170</v>
+        <v>5205956</v>
       </c>
       <c r="C404" t="s">
         <v>28</v>
@@ -36403,76 +36403,76 @@
         <v>44870.54166666666</v>
       </c>
       <c r="F404" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G404" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H404">
         <v>1</v>
       </c>
       <c r="I404">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J404" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K404">
-        <v>2.375</v>
+        <v>5</v>
       </c>
       <c r="L404">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="M404">
-        <v>2.9</v>
+        <v>1.6</v>
       </c>
       <c r="N404">
-        <v>2.3</v>
+        <v>9</v>
       </c>
       <c r="O404">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="P404">
-        <v>3.1</v>
+        <v>1.333</v>
       </c>
       <c r="Q404">
-        <v>-0.25</v>
+        <v>1.5</v>
       </c>
       <c r="R404">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="S404">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="T404">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U404">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V404">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="W404">
         <v>-1</v>
       </c>
       <c r="X404">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y404">
-        <v>-1</v>
+        <v>0.333</v>
       </c>
       <c r="Z404">
+        <v>0.925</v>
+      </c>
+      <c r="AA404">
+        <v>-1</v>
+      </c>
+      <c r="AB404">
         <v>-0.5</v>
       </c>
-      <c r="AA404">
-        <v>0.4375</v>
-      </c>
-      <c r="AB404">
-        <v>-1</v>
-      </c>
       <c r="AC404">
-        <v>0.8500000000000001</v>
+        <v>0.4625</v>
       </c>
     </row>
     <row r="405" spans="1:29">
@@ -37103,7 +37103,7 @@
         <v>410</v>
       </c>
       <c r="B412">
-        <v>5205963</v>
+        <v>5205962</v>
       </c>
       <c r="C412" t="s">
         <v>28</v>
@@ -37115,10 +37115,10 @@
         <v>44878.4375</v>
       </c>
       <c r="F412" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G412" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H412">
         <v>0</v>
@@ -37130,25 +37130,25 @@
         <v>46</v>
       </c>
       <c r="K412">
-        <v>5.25</v>
+        <v>1.909</v>
       </c>
       <c r="L412">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="M412">
-        <v>1.533</v>
+        <v>3.5</v>
       </c>
       <c r="N412">
-        <v>6.5</v>
+        <v>1.85</v>
       </c>
       <c r="O412">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="P412">
-        <v>1.4</v>
+        <v>3.75</v>
       </c>
       <c r="Q412">
-        <v>1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="R412">
         <v>1.875</v>
@@ -37157,13 +37157,13 @@
         <v>1.975</v>
       </c>
       <c r="T412">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U412">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V412">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W412">
         <v>-1</v>
@@ -37172,19 +37172,19 @@
         <v>-1</v>
       </c>
       <c r="Y412">
-        <v>0.3999999999999999</v>
+        <v>2.75</v>
       </c>
       <c r="Z412">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA412">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB412">
         <v>-1</v>
       </c>
       <c r="AC412">
-        <v>1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="413" spans="1:29">
@@ -37192,7 +37192,7 @@
         <v>411</v>
       </c>
       <c r="B413">
-        <v>5205962</v>
+        <v>5205963</v>
       </c>
       <c r="C413" t="s">
         <v>28</v>
@@ -37204,10 +37204,10 @@
         <v>44878.4375</v>
       </c>
       <c r="F413" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G413" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H413">
         <v>0</v>
@@ -37219,25 +37219,25 @@
         <v>46</v>
       </c>
       <c r="K413">
-        <v>1.909</v>
+        <v>5.25</v>
       </c>
       <c r="L413">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="M413">
-        <v>3.5</v>
+        <v>1.533</v>
       </c>
       <c r="N413">
-        <v>1.85</v>
+        <v>6.5</v>
       </c>
       <c r="O413">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="P413">
-        <v>3.75</v>
+        <v>1.4</v>
       </c>
       <c r="Q413">
-        <v>-0.5</v>
+        <v>1.5</v>
       </c>
       <c r="R413">
         <v>1.875</v>
@@ -37246,13 +37246,13 @@
         <v>1.975</v>
       </c>
       <c r="T413">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U413">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V413">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W413">
         <v>-1</v>
@@ -37261,19 +37261,19 @@
         <v>-1</v>
       </c>
       <c r="Y413">
-        <v>2.75</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z413">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA413">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AB413">
         <v>-1</v>
       </c>
       <c r="AC413">
-        <v>1.025</v>
+        <v>1</v>
       </c>
     </row>
     <row r="414" spans="1:29">
@@ -37459,7 +37459,7 @@
         <v>414</v>
       </c>
       <c r="B416">
-        <v>5207168</v>
+        <v>5205966</v>
       </c>
       <c r="C416" t="s">
         <v>28</v>
@@ -37471,49 +37471,49 @@
         <v>44968.54166666666</v>
       </c>
       <c r="F416" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G416" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H416">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I416">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J416" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K416">
-        <v>1.142</v>
+        <v>1.909</v>
       </c>
       <c r="L416">
-        <v>8</v>
+        <v>3.6</v>
       </c>
       <c r="M416">
-        <v>13</v>
+        <v>3.8</v>
       </c>
       <c r="N416">
-        <v>1.2</v>
+        <v>2.15</v>
       </c>
       <c r="O416">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P416">
-        <v>13</v>
+        <v>3.3</v>
       </c>
       <c r="Q416">
-        <v>-2</v>
+        <v>-0.25</v>
       </c>
       <c r="R416">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="S416">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="T416">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U416">
         <v>1.85</v>
@@ -37522,25 +37522,25 @@
         <v>2</v>
       </c>
       <c r="W416">
-        <v>0.2</v>
+        <v>-1</v>
       </c>
       <c r="X416">
         <v>-1</v>
       </c>
       <c r="Y416">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z416">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA416">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB416">
-        <v>0.8500000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="AC416">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="417" spans="1:29">
@@ -37548,7 +37548,7 @@
         <v>415</v>
       </c>
       <c r="B417">
-        <v>5205966</v>
+        <v>5207168</v>
       </c>
       <c r="C417" t="s">
         <v>28</v>
@@ -37560,49 +37560,49 @@
         <v>44968.54166666666</v>
       </c>
       <c r="F417" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G417" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H417">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I417">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J417" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K417">
-        <v>1.909</v>
+        <v>1.142</v>
       </c>
       <c r="L417">
-        <v>3.6</v>
+        <v>8</v>
       </c>
       <c r="M417">
-        <v>3.8</v>
+        <v>13</v>
       </c>
       <c r="N417">
-        <v>2.15</v>
+        <v>1.2</v>
       </c>
       <c r="O417">
+        <v>7.5</v>
+      </c>
+      <c r="P417">
+        <v>13</v>
+      </c>
+      <c r="Q417">
+        <v>-2</v>
+      </c>
+      <c r="R417">
+        <v>1.875</v>
+      </c>
+      <c r="S417">
+        <v>1.975</v>
+      </c>
+      <c r="T417">
         <v>3.5</v>
-      </c>
-      <c r="P417">
-        <v>3.3</v>
-      </c>
-      <c r="Q417">
-        <v>-0.25</v>
-      </c>
-      <c r="R417">
-        <v>1.9</v>
-      </c>
-      <c r="S417">
-        <v>1.95</v>
-      </c>
-      <c r="T417">
-        <v>2.75</v>
       </c>
       <c r="U417">
         <v>1.85</v>
@@ -37611,25 +37611,25 @@
         <v>2</v>
       </c>
       <c r="W417">
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="X417">
         <v>-1</v>
       </c>
       <c r="Y417">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z417">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA417">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB417">
-        <v>0.425</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC417">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="418" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-29 às 23-06
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -33009,7 +33009,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>5205928</v>
+        <v>5205930</v>
       </c>
       <c r="C366" t="s">
         <v>28</v>
@@ -33021,73 +33021,73 @@
         <v>44821.5</v>
       </c>
       <c r="F366" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G366" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H366">
+        <v>1</v>
+      </c>
+      <c r="I366">
+        <v>4</v>
+      </c>
+      <c r="J366" t="s">
+        <v>46</v>
+      </c>
+      <c r="K366">
         <v>3</v>
       </c>
-      <c r="I366">
-        <v>1</v>
-      </c>
-      <c r="J366" t="s">
-        <v>45</v>
-      </c>
-      <c r="K366">
-        <v>1.666</v>
-      </c>
       <c r="L366">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="M366">
-        <v>4.333</v>
+        <v>2.2</v>
       </c>
       <c r="N366">
-        <v>1.727</v>
+        <v>2.8</v>
       </c>
       <c r="O366">
-        <v>4.333</v>
+        <v>3.5</v>
       </c>
       <c r="P366">
-        <v>4</v>
+        <v>2.375</v>
       </c>
       <c r="Q366">
-        <v>-0.75</v>
+        <v>0.25</v>
       </c>
       <c r="R366">
-        <v>1.95</v>
+        <v>1.8</v>
       </c>
       <c r="S366">
-        <v>1.9</v>
+        <v>2.05</v>
       </c>
       <c r="T366">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U366">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="V366">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="W366">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X366">
         <v>-1</v>
       </c>
       <c r="Y366">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Z366">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA366">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB366">
-        <v>0.925</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC366">
         <v>-1</v>
@@ -33098,7 +33098,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>5205927</v>
+        <v>5205928</v>
       </c>
       <c r="C367" t="s">
         <v>28</v>
@@ -33110,73 +33110,73 @@
         <v>44821.5</v>
       </c>
       <c r="F367" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G367" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H367">
+        <v>3</v>
+      </c>
+      <c r="I367">
         <v>1</v>
       </c>
-      <c r="I367">
+      <c r="J367" t="s">
+        <v>45</v>
+      </c>
+      <c r="K367">
+        <v>1.666</v>
+      </c>
+      <c r="L367">
         <v>4</v>
       </c>
-      <c r="J367" t="s">
-        <v>46</v>
-      </c>
-      <c r="K367">
-        <v>1.363</v>
-      </c>
-      <c r="L367">
-        <v>5</v>
-      </c>
       <c r="M367">
-        <v>8</v>
+        <v>4.333</v>
       </c>
       <c r="N367">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="O367">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="P367">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q367">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R367">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S367">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T367">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U367">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V367">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W367">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="X367">
         <v>-1</v>
       </c>
       <c r="Y367">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Z367">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA367">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB367">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="AC367">
         <v>-1</v>
@@ -33187,7 +33187,7 @@
         <v>366</v>
       </c>
       <c r="B368">
-        <v>5205930</v>
+        <v>5205927</v>
       </c>
       <c r="C368" t="s">
         <v>28</v>
@@ -33199,10 +33199,10 @@
         <v>44821.5</v>
       </c>
       <c r="F368" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G368" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H368">
         <v>1</v>
@@ -33214,40 +33214,40 @@
         <v>46</v>
       </c>
       <c r="K368">
-        <v>3</v>
+        <v>1.363</v>
       </c>
       <c r="L368">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="M368">
-        <v>2.2</v>
+        <v>8</v>
       </c>
       <c r="N368">
-        <v>2.8</v>
+        <v>1.5</v>
       </c>
       <c r="O368">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="P368">
-        <v>2.375</v>
+        <v>6</v>
       </c>
       <c r="Q368">
-        <v>0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R368">
+        <v>2.05</v>
+      </c>
+      <c r="S368">
         <v>1.8</v>
       </c>
-      <c r="S368">
-        <v>2.05</v>
-      </c>
       <c r="T368">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U368">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V368">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W368">
         <v>-1</v>
@@ -33256,16 +33256,16 @@
         <v>-1</v>
       </c>
       <c r="Y368">
-        <v>1.375</v>
+        <v>5</v>
       </c>
       <c r="Z368">
         <v>-1</v>
       </c>
       <c r="AA368">
-        <v>1.05</v>
+        <v>0.8</v>
       </c>
       <c r="AB368">
-        <v>0.9750000000000001</v>
+        <v>1.025</v>
       </c>
       <c r="AC368">
         <v>-1</v>
@@ -37459,7 +37459,7 @@
         <v>414</v>
       </c>
       <c r="B416">
-        <v>5205966</v>
+        <v>5207168</v>
       </c>
       <c r="C416" t="s">
         <v>28</v>
@@ -37471,49 +37471,49 @@
         <v>44968.54166666666</v>
       </c>
       <c r="F416" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G416" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H416">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I416">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J416" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K416">
-        <v>1.909</v>
+        <v>1.142</v>
       </c>
       <c r="L416">
-        <v>3.6</v>
+        <v>8</v>
       </c>
       <c r="M416">
-        <v>3.8</v>
+        <v>13</v>
       </c>
       <c r="N416">
-        <v>2.15</v>
+        <v>1.2</v>
       </c>
       <c r="O416">
+        <v>7.5</v>
+      </c>
+      <c r="P416">
+        <v>13</v>
+      </c>
+      <c r="Q416">
+        <v>-2</v>
+      </c>
+      <c r="R416">
+        <v>1.875</v>
+      </c>
+      <c r="S416">
+        <v>1.975</v>
+      </c>
+      <c r="T416">
         <v>3.5</v>
-      </c>
-      <c r="P416">
-        <v>3.3</v>
-      </c>
-      <c r="Q416">
-        <v>-0.25</v>
-      </c>
-      <c r="R416">
-        <v>1.9</v>
-      </c>
-      <c r="S416">
-        <v>1.95</v>
-      </c>
-      <c r="T416">
-        <v>2.75</v>
       </c>
       <c r="U416">
         <v>1.85</v>
@@ -37522,25 +37522,25 @@
         <v>2</v>
       </c>
       <c r="W416">
-        <v>-1</v>
+        <v>0.2</v>
       </c>
       <c r="X416">
         <v>-1</v>
       </c>
       <c r="Y416">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z416">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA416">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB416">
-        <v>0.425</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC416">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="417" spans="1:29">
@@ -37548,7 +37548,7 @@
         <v>415</v>
       </c>
       <c r="B417">
-        <v>5207168</v>
+        <v>5205966</v>
       </c>
       <c r="C417" t="s">
         <v>28</v>
@@ -37560,49 +37560,49 @@
         <v>44968.54166666666</v>
       </c>
       <c r="F417" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G417" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H417">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I417">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J417" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K417">
-        <v>1.142</v>
+        <v>1.909</v>
       </c>
       <c r="L417">
-        <v>8</v>
+        <v>3.6</v>
       </c>
       <c r="M417">
-        <v>13</v>
+        <v>3.8</v>
       </c>
       <c r="N417">
-        <v>1.2</v>
+        <v>2.15</v>
       </c>
       <c r="O417">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P417">
-        <v>13</v>
+        <v>3.3</v>
       </c>
       <c r="Q417">
-        <v>-2</v>
+        <v>-0.25</v>
       </c>
       <c r="R417">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="S417">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="T417">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U417">
         <v>1.85</v>
@@ -37611,25 +37611,25 @@
         <v>2</v>
       </c>
       <c r="W417">
-        <v>0.2</v>
+        <v>-1</v>
       </c>
       <c r="X417">
         <v>-1</v>
       </c>
       <c r="Y417">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z417">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA417">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB417">
-        <v>0.8500000000000001</v>
+        <v>0.425</v>
       </c>
       <c r="AC417">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="418" spans="1:29">
@@ -44045,7 +44045,7 @@
         <v>488</v>
       </c>
       <c r="B490">
-        <v>6429786</v>
+        <v>6430237</v>
       </c>
       <c r="C490" t="s">
         <v>28</v>
@@ -44057,76 +44057,76 @@
         <v>45060.39583333334</v>
       </c>
       <c r="F490" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G490" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H490">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I490">
         <v>1</v>
       </c>
       <c r="J490" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K490">
-        <v>4</v>
+        <v>1.25</v>
       </c>
       <c r="L490">
-        <v>3.6</v>
+        <v>5.5</v>
       </c>
       <c r="M490">
-        <v>1.8</v>
+        <v>10</v>
       </c>
       <c r="N490">
-        <v>3.8</v>
+        <v>1.222</v>
       </c>
       <c r="O490">
-        <v>3.75</v>
+        <v>6.5</v>
       </c>
       <c r="P490">
-        <v>1.95</v>
+        <v>12</v>
       </c>
       <c r="Q490">
-        <v>0.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R490">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="S490">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="T490">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U490">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V490">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W490">
-        <v>-1</v>
+        <v>0.222</v>
       </c>
       <c r="X490">
         <v>-1</v>
       </c>
       <c r="Y490">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z490">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AA490">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB490">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AC490">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="491" spans="1:29">
@@ -44134,7 +44134,7 @@
         <v>489</v>
       </c>
       <c r="B491">
-        <v>6430237</v>
+        <v>6429786</v>
       </c>
       <c r="C491" t="s">
         <v>28</v>
@@ -44146,76 +44146,76 @@
         <v>45060.39583333334</v>
       </c>
       <c r="F491" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G491" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H491">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I491">
         <v>1</v>
       </c>
       <c r="J491" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K491">
-        <v>1.25</v>
+        <v>4</v>
       </c>
       <c r="L491">
-        <v>5.5</v>
+        <v>3.6</v>
       </c>
       <c r="M491">
-        <v>10</v>
+        <v>1.8</v>
       </c>
       <c r="N491">
-        <v>1.222</v>
+        <v>3.8</v>
       </c>
       <c r="O491">
-        <v>6.5</v>
+        <v>3.75</v>
       </c>
       <c r="P491">
-        <v>12</v>
+        <v>1.95</v>
       </c>
       <c r="Q491">
-        <v>-1.75</v>
+        <v>0.5</v>
       </c>
       <c r="R491">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="S491">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="T491">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U491">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V491">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W491">
-        <v>0.222</v>
+        <v>-1</v>
       </c>
       <c r="X491">
         <v>-1</v>
       </c>
       <c r="Y491">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z491">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AA491">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB491">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC491">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="492" spans="1:29">
@@ -44401,7 +44401,7 @@
         <v>492</v>
       </c>
       <c r="B494">
-        <v>6430222</v>
+        <v>6430223</v>
       </c>
       <c r="C494" t="s">
         <v>28</v>
@@ -44413,55 +44413,55 @@
         <v>45066.5</v>
       </c>
       <c r="F494" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G494" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="H494">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I494">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J494" t="s">
         <v>46</v>
       </c>
       <c r="K494">
-        <v>2.2</v>
+        <v>2.45</v>
       </c>
       <c r="L494">
         <v>3.4</v>
       </c>
       <c r="M494">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="N494">
-        <v>1.95</v>
+        <v>2.9</v>
       </c>
       <c r="O494">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P494">
-        <v>3.75</v>
+        <v>2.375</v>
       </c>
       <c r="Q494">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R494">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S494">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T494">
         <v>2.75</v>
       </c>
       <c r="U494">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V494">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W494">
         <v>-1</v>
@@ -44470,19 +44470,19 @@
         <v>-1</v>
       </c>
       <c r="Y494">
-        <v>2.75</v>
+        <v>1.375</v>
       </c>
       <c r="Z494">
         <v>-1</v>
       </c>
       <c r="AA494">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
       <c r="AB494">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC494">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="495" spans="1:29">
@@ -44490,7 +44490,7 @@
         <v>493</v>
       </c>
       <c r="B495">
-        <v>6430223</v>
+        <v>6430222</v>
       </c>
       <c r="C495" t="s">
         <v>28</v>
@@ -44502,55 +44502,55 @@
         <v>45066.5</v>
       </c>
       <c r="F495" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G495" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H495">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I495">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J495" t="s">
         <v>46</v>
       </c>
       <c r="K495">
-        <v>2.45</v>
+        <v>2.2</v>
       </c>
       <c r="L495">
         <v>3.4</v>
       </c>
       <c r="M495">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="N495">
-        <v>2.9</v>
+        <v>1.95</v>
       </c>
       <c r="O495">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="P495">
-        <v>2.375</v>
+        <v>3.75</v>
       </c>
       <c r="Q495">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R495">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S495">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T495">
         <v>2.75</v>
       </c>
       <c r="U495">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V495">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W495">
         <v>-1</v>
@@ -44559,19 +44559,19 @@
         <v>-1</v>
       </c>
       <c r="Y495">
-        <v>1.375</v>
+        <v>2.75</v>
       </c>
       <c r="Z495">
         <v>-1</v>
       </c>
       <c r="AA495">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="AB495">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC495">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="496" spans="1:29">
@@ -45380,7 +45380,7 @@
         <v>503</v>
       </c>
       <c r="B505">
-        <v>6430227</v>
+        <v>6430229</v>
       </c>
       <c r="C505" t="s">
         <v>28</v>
@@ -45392,76 +45392,76 @@
         <v>45079.60416666666</v>
       </c>
       <c r="F505" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G505" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H505">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I505">
         <v>1</v>
       </c>
       <c r="J505" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K505">
-        <v>2.625</v>
+        <v>1.8</v>
       </c>
       <c r="L505">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="M505">
-        <v>2.55</v>
+        <v>4.2</v>
       </c>
       <c r="N505">
+        <v>1.909</v>
+      </c>
+      <c r="O505">
         <v>3.75</v>
       </c>
-      <c r="O505">
-        <v>3.6</v>
-      </c>
       <c r="P505">
+        <v>3.8</v>
+      </c>
+      <c r="Q505">
+        <v>-0.5</v>
+      </c>
+      <c r="R505">
         <v>1.95</v>
       </c>
-      <c r="Q505">
-        <v>0.5</v>
-      </c>
-      <c r="R505">
-        <v>1.875</v>
-      </c>
       <c r="S505">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="T505">
+        <v>3.25</v>
+      </c>
+      <c r="U505">
+        <v>2.025</v>
+      </c>
+      <c r="V505">
+        <v>1.825</v>
+      </c>
+      <c r="W505">
+        <v>-1</v>
+      </c>
+      <c r="X505">
         <v>2.75</v>
       </c>
-      <c r="U505">
-        <v>1.9</v>
-      </c>
-      <c r="V505">
-        <v>1.95</v>
-      </c>
-      <c r="W505">
-        <v>2.75</v>
-      </c>
-      <c r="X505">
-        <v>-1</v>
-      </c>
       <c r="Y505">
         <v>-1</v>
       </c>
       <c r="Z505">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA505">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AB505">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC505">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="506" spans="1:29">
@@ -45469,7 +45469,7 @@
         <v>504</v>
       </c>
       <c r="B506">
-        <v>6430228</v>
+        <v>6430227</v>
       </c>
       <c r="C506" t="s">
         <v>28</v>
@@ -45481,76 +45481,76 @@
         <v>45079.60416666666</v>
       </c>
       <c r="F506" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G506" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H506">
+        <v>5</v>
+      </c>
+      <c r="I506">
         <v>1</v>
       </c>
-      <c r="I506">
-        <v>2</v>
-      </c>
       <c r="J506" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K506">
-        <v>2.55</v>
+        <v>2.625</v>
       </c>
       <c r="L506">
         <v>3.4</v>
       </c>
       <c r="M506">
-        <v>2.625</v>
+        <v>2.55</v>
       </c>
       <c r="N506">
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
       <c r="O506">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P506">
-        <v>2.3</v>
+        <v>1.95</v>
       </c>
       <c r="Q506">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R506">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="S506">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="T506">
         <v>2.75</v>
       </c>
       <c r="U506">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V506">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W506">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="X506">
         <v>-1</v>
       </c>
       <c r="Y506">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z506">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA506">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB506">
-        <v>0.4625</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC506">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="507" spans="1:29">
@@ -45558,7 +45558,7 @@
         <v>505</v>
       </c>
       <c r="B507">
-        <v>6430229</v>
+        <v>6430228</v>
       </c>
       <c r="C507" t="s">
         <v>28</v>
@@ -45570,76 +45570,76 @@
         <v>45079.60416666666</v>
       </c>
       <c r="F507" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G507" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H507">
         <v>1</v>
       </c>
       <c r="I507">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J507" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K507">
-        <v>1.8</v>
+        <v>2.55</v>
       </c>
       <c r="L507">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="M507">
-        <v>4.2</v>
+        <v>2.625</v>
       </c>
       <c r="N507">
-        <v>1.909</v>
+        <v>2.8</v>
       </c>
       <c r="O507">
-        <v>3.75</v>
+        <v>3.8</v>
       </c>
       <c r="P507">
-        <v>3.8</v>
+        <v>2.3</v>
       </c>
       <c r="Q507">
+        <v>0.25</v>
+      </c>
+      <c r="R507">
+        <v>1.825</v>
+      </c>
+      <c r="S507">
+        <v>2.025</v>
+      </c>
+      <c r="T507">
+        <v>2.75</v>
+      </c>
+      <c r="U507">
+        <v>1.925</v>
+      </c>
+      <c r="V507">
+        <v>1.925</v>
+      </c>
+      <c r="W507">
+        <v>-1</v>
+      </c>
+      <c r="X507">
+        <v>-1</v>
+      </c>
+      <c r="Y507">
+        <v>1.3</v>
+      </c>
+      <c r="Z507">
+        <v>-1</v>
+      </c>
+      <c r="AA507">
+        <v>1.025</v>
+      </c>
+      <c r="AB507">
+        <v>0.4625</v>
+      </c>
+      <c r="AC507">
         <v>-0.5</v>
-      </c>
-      <c r="R507">
-        <v>1.95</v>
-      </c>
-      <c r="S507">
-        <v>1.9</v>
-      </c>
-      <c r="T507">
-        <v>3.25</v>
-      </c>
-      <c r="U507">
-        <v>2.025</v>
-      </c>
-      <c r="V507">
-        <v>1.825</v>
-      </c>
-      <c r="W507">
-        <v>-1</v>
-      </c>
-      <c r="X507">
-        <v>2.75</v>
-      </c>
-      <c r="Y507">
-        <v>-1</v>
-      </c>
-      <c r="Z507">
-        <v>-1</v>
-      </c>
-      <c r="AA507">
-        <v>0.8999999999999999</v>
-      </c>
-      <c r="AB507">
-        <v>-1</v>
-      </c>
-      <c r="AC507">
-        <v>0.825</v>
       </c>
     </row>
     <row r="508" spans="1:29">
@@ -46003,7 +46003,7 @@
         <v>510</v>
       </c>
       <c r="B512">
-        <v>6851964</v>
+        <v>6847027</v>
       </c>
       <c r="C512" t="s">
         <v>28</v>
@@ -46015,73 +46015,73 @@
         <v>45136.5</v>
       </c>
       <c r="F512" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G512" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H512">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I512">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J512" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K512">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="L512">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="M512">
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="N512">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="O512">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="P512">
-        <v>3.25</v>
+        <v>2.8</v>
       </c>
       <c r="Q512">
         <v>-0.25</v>
       </c>
       <c r="R512">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="S512">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="T512">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U512">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="V512">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W512">
-        <v>1.2</v>
+        <v>-1</v>
       </c>
       <c r="X512">
         <v>-1</v>
       </c>
       <c r="Y512">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z512">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA512">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB512">
-        <v>1</v>
+        <v>0.825</v>
       </c>
       <c r="AC512">
         <v>-1</v>
@@ -46092,7 +46092,7 @@
         <v>511</v>
       </c>
       <c r="B513">
-        <v>6847027</v>
+        <v>6851964</v>
       </c>
       <c r="C513" t="s">
         <v>28</v>
@@ -46104,73 +46104,73 @@
         <v>45136.5</v>
       </c>
       <c r="F513" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="G513" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H513">
+        <v>2</v>
+      </c>
+      <c r="I513">
         <v>1</v>
       </c>
-      <c r="I513">
-        <v>3</v>
-      </c>
       <c r="J513" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K513">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="L513">
+        <v>3.5</v>
+      </c>
+      <c r="M513">
+        <v>3.5</v>
+      </c>
+      <c r="N513">
+        <v>2.2</v>
+      </c>
+      <c r="O513">
         <v>3.4</v>
       </c>
-      <c r="M513">
-        <v>3.1</v>
-      </c>
-      <c r="N513">
-        <v>2.3</v>
-      </c>
-      <c r="O513">
-        <v>3.6</v>
-      </c>
       <c r="P513">
-        <v>2.8</v>
+        <v>3.25</v>
       </c>
       <c r="Q513">
         <v>-0.25</v>
       </c>
       <c r="R513">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="S513">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="T513">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="U513">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V513">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W513">
-        <v>-1</v>
+        <v>1.2</v>
       </c>
       <c r="X513">
         <v>-1</v>
       </c>
       <c r="Y513">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z513">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA513">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB513">
-        <v>0.825</v>
+        <v>1</v>
       </c>
       <c r="AC513">
         <v>-1</v>
@@ -46626,7 +46626,7 @@
         <v>517</v>
       </c>
       <c r="B519">
-        <v>6851963</v>
+        <v>6847032</v>
       </c>
       <c r="C519" t="s">
         <v>28</v>
@@ -46638,40 +46638,40 @@
         <v>45144.5</v>
       </c>
       <c r="F519" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G519" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H519">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I519">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J519" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K519">
-        <v>2.7</v>
+        <v>4.2</v>
       </c>
       <c r="L519">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="M519">
-        <v>2.55</v>
+        <v>1.75</v>
       </c>
       <c r="N519">
-        <v>2.25</v>
+        <v>3.75</v>
       </c>
       <c r="O519">
-        <v>3.5</v>
+        <v>3.8</v>
       </c>
       <c r="P519">
-        <v>3.1</v>
+        <v>1.909</v>
       </c>
       <c r="Q519">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R519">
         <v>1.975</v>
@@ -46680,34 +46680,34 @@
         <v>1.875</v>
       </c>
       <c r="T519">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U519">
+        <v>1.95</v>
+      </c>
+      <c r="V519">
         <v>1.9</v>
       </c>
-      <c r="V519">
-        <v>1.95</v>
-      </c>
       <c r="W519">
         <v>-1</v>
       </c>
       <c r="X519">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y519">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="Z519">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AA519">
-        <v>0.4375</v>
+        <v>0.875</v>
       </c>
       <c r="AB519">
+        <v>-1</v>
+      </c>
+      <c r="AC519">
         <v>0.8999999999999999</v>
-      </c>
-      <c r="AC519">
-        <v>-1</v>
       </c>
     </row>
     <row r="520" spans="1:29">
@@ -46715,7 +46715,7 @@
         <v>518</v>
       </c>
       <c r="B520">
-        <v>6847032</v>
+        <v>6846459</v>
       </c>
       <c r="C520" t="s">
         <v>28</v>
@@ -46727,76 +46727,76 @@
         <v>45144.5</v>
       </c>
       <c r="F520" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G520" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H520">
+        <v>3</v>
+      </c>
+      <c r="I520">
         <v>0</v>
       </c>
-      <c r="I520">
-        <v>2</v>
-      </c>
       <c r="J520" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K520">
-        <v>4.2</v>
+        <v>1.142</v>
       </c>
       <c r="L520">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M520">
-        <v>1.75</v>
+        <v>17</v>
       </c>
       <c r="N520">
+        <v>1.166</v>
+      </c>
+      <c r="O520">
+        <v>7.5</v>
+      </c>
+      <c r="P520">
+        <v>15</v>
+      </c>
+      <c r="Q520">
+        <v>-2.25</v>
+      </c>
+      <c r="R520">
+        <v>1.95</v>
+      </c>
+      <c r="S520">
+        <v>1.9</v>
+      </c>
+      <c r="T520">
         <v>3.75</v>
       </c>
-      <c r="O520">
-        <v>3.8</v>
-      </c>
-      <c r="P520">
-        <v>1.909</v>
-      </c>
-      <c r="Q520">
-        <v>0.5</v>
-      </c>
-      <c r="R520">
-        <v>1.975</v>
-      </c>
-      <c r="S520">
-        <v>1.875</v>
-      </c>
-      <c r="T520">
-        <v>3</v>
-      </c>
       <c r="U520">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V520">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W520">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="X520">
         <v>-1</v>
       </c>
       <c r="Y520">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="Z520">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA520">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB520">
         <v>-1</v>
       </c>
       <c r="AC520">
-        <v>0.8999999999999999</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="521" spans="1:29">
@@ -46804,7 +46804,7 @@
         <v>519</v>
       </c>
       <c r="B521">
-        <v>6846459</v>
+        <v>6851963</v>
       </c>
       <c r="C521" t="s">
         <v>28</v>
@@ -46816,76 +46816,76 @@
         <v>45144.5</v>
       </c>
       <c r="F521" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G521" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H521">
         <v>3</v>
       </c>
       <c r="I521">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J521" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K521">
-        <v>1.142</v>
+        <v>2.7</v>
       </c>
       <c r="L521">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="M521">
-        <v>17</v>
+        <v>2.55</v>
       </c>
       <c r="N521">
-        <v>1.166</v>
+        <v>2.25</v>
       </c>
       <c r="O521">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P521">
-        <v>15</v>
+        <v>3.1</v>
       </c>
       <c r="Q521">
-        <v>-2.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R521">
+        <v>1.975</v>
+      </c>
+      <c r="S521">
+        <v>1.875</v>
+      </c>
+      <c r="T521">
+        <v>2.75</v>
+      </c>
+      <c r="U521">
+        <v>1.9</v>
+      </c>
+      <c r="V521">
         <v>1.95</v>
       </c>
-      <c r="S521">
-        <v>1.9</v>
-      </c>
-      <c r="T521">
-        <v>3.75</v>
-      </c>
-      <c r="U521">
-        <v>1.925</v>
-      </c>
-      <c r="V521">
-        <v>1.925</v>
-      </c>
       <c r="W521">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X521">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y521">
         <v>-1</v>
       </c>
       <c r="Z521">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA521">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AB521">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC521">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="522" spans="1:29">
@@ -50453,7 +50453,7 @@
         <v>560</v>
       </c>
       <c r="B562">
-        <v>6847061</v>
+        <v>6847060</v>
       </c>
       <c r="C562" t="s">
         <v>28</v>
@@ -50465,61 +50465,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F562" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G562" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H562">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I562">
         <v>0</v>
       </c>
       <c r="J562" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K562">
-        <v>1.909</v>
+        <v>1.25</v>
       </c>
       <c r="L562">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="M562">
-        <v>3.9</v>
+        <v>10</v>
       </c>
       <c r="N562">
-        <v>2</v>
+        <v>1.285</v>
       </c>
       <c r="O562">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
       <c r="P562">
-        <v>3.6</v>
+        <v>9</v>
       </c>
       <c r="Q562">
-        <v>-0.5</v>
+        <v>-1.75</v>
       </c>
       <c r="R562">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="S562">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="T562">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="U562">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V562">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="W562">
-        <v>-1</v>
+        <v>0.2849999999999999</v>
       </c>
       <c r="X562">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y562">
         <v>-1</v>
@@ -50528,13 +50528,13 @@
         <v>-1</v>
       </c>
       <c r="AA562">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AB562">
         <v>-1</v>
       </c>
       <c r="AC562">
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="563" spans="1:29">
@@ -50542,7 +50542,7 @@
         <v>561</v>
       </c>
       <c r="B563">
-        <v>6847060</v>
+        <v>6847061</v>
       </c>
       <c r="C563" t="s">
         <v>28</v>
@@ -50554,61 +50554,61 @@
         <v>45200.39583333334</v>
       </c>
       <c r="F563" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G563" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H563">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I563">
         <v>0</v>
       </c>
       <c r="J563" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K563">
-        <v>1.25</v>
+        <v>1.909</v>
       </c>
       <c r="L563">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M563">
-        <v>10</v>
+        <v>3.9</v>
       </c>
       <c r="N563">
-        <v>1.285</v>
+        <v>2</v>
       </c>
       <c r="O563">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="P563">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="Q563">
-        <v>-1.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R563">
-        <v>1.925</v>
+        <v>2.05</v>
       </c>
       <c r="S563">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="T563">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="U563">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="V563">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="W563">
-        <v>0.2849999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X563">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y563">
         <v>-1</v>
@@ -50617,13 +50617,13 @@
         <v>-1</v>
       </c>
       <c r="AA563">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AB563">
         <v>-1</v>
       </c>
       <c r="AC563">
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="564" spans="1:29">
@@ -51254,7 +51254,7 @@
         <v>569</v>
       </c>
       <c r="B571">
-        <v>6847066</v>
+        <v>6851954</v>
       </c>
       <c r="C571" t="s">
         <v>28</v>
@@ -51266,76 +51266,76 @@
         <v>45220.5</v>
       </c>
       <c r="F571" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G571" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H571">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I571">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J571" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K571">
-        <v>1.5</v>
+        <v>2.05</v>
       </c>
       <c r="L571">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="M571">
-        <v>5.5</v>
+        <v>3.2</v>
       </c>
       <c r="N571">
-        <v>1.7</v>
+        <v>1.666</v>
       </c>
       <c r="O571">
         <v>4</v>
       </c>
       <c r="P571">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="Q571">
         <v>-0.75</v>
       </c>
       <c r="R571">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="S571">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="T571">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U571">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="V571">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="W571">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="X571">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="Y571">
         <v>-1</v>
       </c>
       <c r="Z571">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AA571">
-        <v>-0.5</v>
+        <v>1.025</v>
       </c>
       <c r="AB571">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC571">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="572" spans="1:29">
@@ -51343,7 +51343,7 @@
         <v>570</v>
       </c>
       <c r="B572">
-        <v>6851954</v>
+        <v>6847066</v>
       </c>
       <c r="C572" t="s">
         <v>28</v>
@@ -51355,76 +51355,76 @@
         <v>45220.5</v>
       </c>
       <c r="F572" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G572" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H572">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I572">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J572" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K572">
-        <v>2.05</v>
+        <v>1.5</v>
       </c>
       <c r="L572">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="M572">
-        <v>3.2</v>
+        <v>5.5</v>
       </c>
       <c r="N572">
-        <v>1.666</v>
+        <v>1.7</v>
       </c>
       <c r="O572">
         <v>4</v>
       </c>
       <c r="P572">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="Q572">
         <v>-0.75</v>
       </c>
       <c r="R572">
+        <v>1.925</v>
+      </c>
+      <c r="S572">
+        <v>1.925</v>
+      </c>
+      <c r="T572">
+        <v>2.5</v>
+      </c>
+      <c r="U572">
         <v>1.825</v>
       </c>
-      <c r="S572">
+      <c r="V572">
         <v>2.025</v>
       </c>
-      <c r="T572">
-        <v>2.75</v>
-      </c>
-      <c r="U572">
-        <v>1.875</v>
-      </c>
-      <c r="V572">
-        <v>1.975</v>
-      </c>
       <c r="W572">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="X572">
-        <v>3</v>
+        <v>-1</v>
       </c>
       <c r="Y572">
         <v>-1</v>
       </c>
       <c r="Z572">
-        <v>-1</v>
+        <v>0.4625</v>
       </c>
       <c r="AA572">
-        <v>1.025</v>
+        <v>-0.5</v>
       </c>
       <c r="AB572">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC572">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="573" spans="1:29">

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-01-31 às 20-02
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -30428,7 +30428,7 @@
         <v>335</v>
       </c>
       <c r="B337">
-        <v>5205901</v>
+        <v>5205902</v>
       </c>
       <c r="C337" t="s">
         <v>28</v>
@@ -30440,40 +30440,40 @@
         <v>44786.5</v>
       </c>
       <c r="F337" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G337" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H337">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I337">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J337" t="s">
         <v>45</v>
       </c>
       <c r="K337">
-        <v>1.7</v>
+        <v>2.5</v>
       </c>
       <c r="L337">
-        <v>4</v>
+        <v>3.4</v>
       </c>
       <c r="M337">
-        <v>4.333</v>
+        <v>2.7</v>
       </c>
       <c r="N337">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="O337">
-        <v>4.5</v>
+        <v>3.6</v>
       </c>
       <c r="P337">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="Q337">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="R337">
         <v>2.025</v>
@@ -30482,7 +30482,7 @@
         <v>1.825</v>
       </c>
       <c r="T337">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U337">
         <v>1.85</v>
@@ -30491,7 +30491,7 @@
         <v>2</v>
       </c>
       <c r="W337">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="X337">
         <v>-1</v>
@@ -30500,16 +30500,16 @@
         <v>-1</v>
       </c>
       <c r="Z337">
-        <v>0.5125</v>
+        <v>1.025</v>
       </c>
       <c r="AA337">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AB337">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AC337">
-        <v>-0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="338" spans="1:29">
@@ -30517,7 +30517,7 @@
         <v>336</v>
       </c>
       <c r="B338">
-        <v>5205902</v>
+        <v>5205901</v>
       </c>
       <c r="C338" t="s">
         <v>28</v>
@@ -30529,40 +30529,40 @@
         <v>44786.5</v>
       </c>
       <c r="F338" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G338" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H338">
+        <v>2</v>
+      </c>
+      <c r="I338">
         <v>1</v>
-      </c>
-      <c r="I338">
-        <v>0</v>
       </c>
       <c r="J338" t="s">
         <v>45</v>
       </c>
       <c r="K338">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="L338">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="M338">
-        <v>2.7</v>
+        <v>4.333</v>
       </c>
       <c r="N338">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="O338">
-        <v>3.6</v>
+        <v>4.5</v>
       </c>
       <c r="P338">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="Q338">
-        <v>-0.5</v>
+        <v>-0.75</v>
       </c>
       <c r="R338">
         <v>2.025</v>
@@ -30571,7 +30571,7 @@
         <v>1.825</v>
       </c>
       <c r="T338">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="U338">
         <v>1.85</v>
@@ -30580,7 +30580,7 @@
         <v>2</v>
       </c>
       <c r="W338">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="X338">
         <v>-1</v>
@@ -30589,16 +30589,16 @@
         <v>-1</v>
       </c>
       <c r="Z338">
-        <v>1.025</v>
+        <v>0.5125</v>
       </c>
       <c r="AA338">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB338">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AC338">
-        <v>1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="339" spans="1:29">
@@ -30695,7 +30695,7 @@
         <v>338</v>
       </c>
       <c r="B340">
-        <v>5207181</v>
+        <v>5205904</v>
       </c>
       <c r="C340" t="s">
         <v>28</v>
@@ -30707,13 +30707,13 @@
         <v>44787.5</v>
       </c>
       <c r="F340" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G340" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H340">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I340">
         <v>1</v>
@@ -30722,25 +30722,25 @@
         <v>45</v>
       </c>
       <c r="K340">
-        <v>2.375</v>
+        <v>1.285</v>
       </c>
       <c r="L340">
-        <v>3.4</v>
+        <v>6.5</v>
       </c>
       <c r="M340">
-        <v>2.875</v>
+        <v>8</v>
       </c>
       <c r="N340">
-        <v>2.3</v>
+        <v>1.25</v>
       </c>
       <c r="O340">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="P340">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="Q340">
-        <v>-0.25</v>
+        <v>-2</v>
       </c>
       <c r="R340">
         <v>2.05</v>
@@ -30749,16 +30749,16 @@
         <v>1.8</v>
       </c>
       <c r="T340">
-        <v>2.75</v>
+        <v>3.5</v>
       </c>
       <c r="U340">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V340">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W340">
-        <v>1.3</v>
+        <v>0.25</v>
       </c>
       <c r="X340">
         <v>-1</v>
@@ -30767,16 +30767,16 @@
         <v>-1</v>
       </c>
       <c r="Z340">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="AA340">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB340">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AC340">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="341" spans="1:29">
@@ -30784,7 +30784,7 @@
         <v>339</v>
       </c>
       <c r="B341">
-        <v>5205904</v>
+        <v>5207181</v>
       </c>
       <c r="C341" t="s">
         <v>28</v>
@@ -30796,13 +30796,13 @@
         <v>44787.5</v>
       </c>
       <c r="F341" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="G341" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H341">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I341">
         <v>1</v>
@@ -30811,25 +30811,25 @@
         <v>45</v>
       </c>
       <c r="K341">
-        <v>1.285</v>
+        <v>2.375</v>
       </c>
       <c r="L341">
-        <v>6.5</v>
+        <v>3.4</v>
       </c>
       <c r="M341">
-        <v>8</v>
+        <v>2.875</v>
       </c>
       <c r="N341">
-        <v>1.25</v>
+        <v>2.3</v>
       </c>
       <c r="O341">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P341">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="Q341">
-        <v>-2</v>
+        <v>-0.25</v>
       </c>
       <c r="R341">
         <v>2.05</v>
@@ -30838,16 +30838,16 @@
         <v>1.8</v>
       </c>
       <c r="T341">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="U341">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="V341">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W341">
-        <v>0.25</v>
+        <v>1.3</v>
       </c>
       <c r="X341">
         <v>-1</v>
@@ -30856,16 +30856,16 @@
         <v>-1</v>
       </c>
       <c r="Z341">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AA341">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB341">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AC341">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="342" spans="1:29">
@@ -31229,7 +31229,7 @@
         <v>344</v>
       </c>
       <c r="B346">
-        <v>5205909</v>
+        <v>5205910</v>
       </c>
       <c r="C346" t="s">
         <v>28</v>
@@ -31241,10 +31241,10 @@
         <v>44794.5</v>
       </c>
       <c r="F346" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G346" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H346">
         <v>1</v>
@@ -31256,40 +31256,40 @@
         <v>46</v>
       </c>
       <c r="K346">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="L346">
         <v>3.25</v>
       </c>
       <c r="M346">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="N346">
-        <v>2.7</v>
+        <v>2.375</v>
       </c>
       <c r="O346">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="P346">
-        <v>2.5</v>
+        <v>3.1</v>
       </c>
       <c r="Q346">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="R346">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="S346">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="T346">
         <v>2.75</v>
       </c>
       <c r="U346">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="V346">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="W346">
         <v>-1</v>
@@ -31298,16 +31298,16 @@
         <v>-1</v>
       </c>
       <c r="Y346">
-        <v>1.5</v>
+        <v>2.1</v>
       </c>
       <c r="Z346">
         <v>-1</v>
       </c>
       <c r="AA346">
-        <v>0.825</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB346">
-        <v>0.4375</v>
+        <v>0.4625</v>
       </c>
       <c r="AC346">
         <v>-0.5</v>
@@ -31318,7 +31318,7 @@
         <v>345</v>
       </c>
       <c r="B347">
-        <v>5205910</v>
+        <v>5205909</v>
       </c>
       <c r="C347" t="s">
         <v>28</v>
@@ -31330,10 +31330,10 @@
         <v>44794.5</v>
       </c>
       <c r="F347" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G347" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H347">
         <v>1</v>
@@ -31345,40 +31345,40 @@
         <v>46</v>
       </c>
       <c r="K347">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="L347">
         <v>3.25</v>
       </c>
       <c r="M347">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="N347">
-        <v>2.375</v>
+        <v>2.7</v>
       </c>
       <c r="O347">
-        <v>3.3</v>
+        <v>3.5</v>
       </c>
       <c r="P347">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="Q347">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="R347">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="S347">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="T347">
         <v>2.75</v>
       </c>
       <c r="U347">
-        <v>1.925</v>
+        <v>1.875</v>
       </c>
       <c r="V347">
-        <v>1.925</v>
+        <v>1.975</v>
       </c>
       <c r="W347">
         <v>-1</v>
@@ -31387,16 +31387,16 @@
         <v>-1</v>
       </c>
       <c r="Y347">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="Z347">
         <v>-1</v>
       </c>
       <c r="AA347">
-        <v>0.8500000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB347">
-        <v>0.4625</v>
+        <v>0.4375</v>
       </c>
       <c r="AC347">
         <v>-0.5</v>
@@ -32475,7 +32475,7 @@
         <v>358</v>
       </c>
       <c r="B360">
-        <v>5205923</v>
+        <v>5205922</v>
       </c>
       <c r="C360" t="s">
         <v>28</v>
@@ -32487,13 +32487,13 @@
         <v>44814.5</v>
       </c>
       <c r="F360" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G360" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H360">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I360">
         <v>3</v>
@@ -32502,40 +32502,40 @@
         <v>46</v>
       </c>
       <c r="K360">
-        <v>7.5</v>
+        <v>2.1</v>
       </c>
       <c r="L360">
-        <v>5.5</v>
+        <v>3.5</v>
       </c>
       <c r="M360">
-        <v>1.333</v>
+        <v>3.4</v>
       </c>
       <c r="N360">
-        <v>6.5</v>
+        <v>2</v>
       </c>
       <c r="O360">
-        <v>4.5</v>
+        <v>3.75</v>
       </c>
       <c r="P360">
-        <v>1.45</v>
+        <v>3.5</v>
       </c>
       <c r="Q360">
-        <v>1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R360">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="S360">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="T360">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U360">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="V360">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="W360">
         <v>-1</v>
@@ -32544,19 +32544,19 @@
         <v>-1</v>
       </c>
       <c r="Y360">
-        <v>0.45</v>
+        <v>2.5</v>
       </c>
       <c r="Z360">
         <v>-1</v>
       </c>
       <c r="AA360">
-        <v>0.9750000000000001</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB360">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AC360">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="361" spans="1:29">
@@ -32564,7 +32564,7 @@
         <v>359</v>
       </c>
       <c r="B361">
-        <v>5205922</v>
+        <v>5205923</v>
       </c>
       <c r="C361" t="s">
         <v>28</v>
@@ -32576,13 +32576,13 @@
         <v>44814.5</v>
       </c>
       <c r="F361" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G361" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H361">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I361">
         <v>3</v>
@@ -32591,40 +32591,40 @@
         <v>46</v>
       </c>
       <c r="K361">
-        <v>2.1</v>
+        <v>7.5</v>
       </c>
       <c r="L361">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="M361">
-        <v>3.4</v>
+        <v>1.333</v>
       </c>
       <c r="N361">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="O361">
-        <v>3.75</v>
+        <v>4.5</v>
       </c>
       <c r="P361">
-        <v>3.5</v>
+        <v>1.45</v>
       </c>
       <c r="Q361">
-        <v>-0.5</v>
+        <v>1.25</v>
       </c>
       <c r="R361">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="S361">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="T361">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U361">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="V361">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="W361">
         <v>-1</v>
@@ -32633,19 +32633,19 @@
         <v>-1</v>
       </c>
       <c r="Y361">
-        <v>2.5</v>
+        <v>0.45</v>
       </c>
       <c r="Z361">
         <v>-1</v>
       </c>
       <c r="AA361">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB361">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AC361">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="362" spans="1:29">
@@ -33009,7 +33009,7 @@
         <v>364</v>
       </c>
       <c r="B366">
-        <v>5205928</v>
+        <v>5205927</v>
       </c>
       <c r="C366" t="s">
         <v>28</v>
@@ -33021,73 +33021,73 @@
         <v>44821.5</v>
       </c>
       <c r="F366" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G366" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H366">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I366">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J366" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K366">
-        <v>1.666</v>
+        <v>1.363</v>
       </c>
       <c r="L366">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M366">
-        <v>4.333</v>
+        <v>8</v>
       </c>
       <c r="N366">
-        <v>1.727</v>
+        <v>1.5</v>
       </c>
       <c r="O366">
-        <v>4.333</v>
+        <v>4.75</v>
       </c>
       <c r="P366">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q366">
-        <v>-0.75</v>
+        <v>-1.25</v>
       </c>
       <c r="R366">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="S366">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="T366">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U366">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="V366">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="W366">
-        <v>0.7270000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X366">
         <v>-1</v>
       </c>
       <c r="Y366">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Z366">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA366">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AB366">
-        <v>0.925</v>
+        <v>1.025</v>
       </c>
       <c r="AC366">
         <v>-1</v>
@@ -33098,7 +33098,7 @@
         <v>365</v>
       </c>
       <c r="B367">
-        <v>5205927</v>
+        <v>5205928</v>
       </c>
       <c r="C367" t="s">
         <v>28</v>
@@ -33110,73 +33110,73 @@
         <v>44821.5</v>
       </c>
       <c r="F367" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G367" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H367">
+        <v>3</v>
+      </c>
+      <c r="I367">
         <v>1</v>
       </c>
-      <c r="I367">
+      <c r="J367" t="s">
+        <v>45</v>
+      </c>
+      <c r="K367">
+        <v>1.666</v>
+      </c>
+      <c r="L367">
         <v>4</v>
       </c>
-      <c r="J367" t="s">
-        <v>46</v>
-      </c>
-      <c r="K367">
-        <v>1.363</v>
-      </c>
-      <c r="L367">
-        <v>5</v>
-      </c>
       <c r="M367">
-        <v>8</v>
+        <v>4.333</v>
       </c>
       <c r="N367">
-        <v>1.5</v>
+        <v>1.727</v>
       </c>
       <c r="O367">
-        <v>4.75</v>
+        <v>4.333</v>
       </c>
       <c r="P367">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q367">
-        <v>-1.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R367">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="S367">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="T367">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U367">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="V367">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="W367">
-        <v>-1</v>
+        <v>0.7270000000000001</v>
       </c>
       <c r="X367">
         <v>-1</v>
       </c>
       <c r="Y367">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Z367">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA367">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AB367">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="AC367">
         <v>-1</v>
@@ -49741,7 +49741,7 @@
         <v>552</v>
       </c>
       <c r="B554">
-        <v>6851957</v>
+        <v>6847054</v>
       </c>
       <c r="C554" t="s">
         <v>28</v>
@@ -49753,76 +49753,76 @@
         <v>45192.5</v>
       </c>
       <c r="F554" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G554" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H554">
+        <v>1</v>
+      </c>
+      <c r="I554">
         <v>0</v>
       </c>
-      <c r="I554">
-        <v>1</v>
-      </c>
       <c r="J554" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K554">
-        <v>1.181</v>
+        <v>1.95</v>
       </c>
       <c r="L554">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="M554">
-        <v>12</v>
+        <v>3.75</v>
       </c>
       <c r="N554">
-        <v>1.25</v>
+        <v>1.65</v>
       </c>
       <c r="O554">
-        <v>7.5</v>
+        <v>4</v>
       </c>
       <c r="P554">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q554">
-        <v>-1.75</v>
+        <v>-0.75</v>
       </c>
       <c r="R554">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="S554">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="T554">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U554">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="V554">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="W554">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="X554">
         <v>-1</v>
       </c>
       <c r="Y554">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="Z554">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AA554">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="AB554">
         <v>-1</v>
       </c>
       <c r="AC554">
-        <v>0.825</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="555" spans="1:29">
@@ -49830,7 +49830,7 @@
         <v>553</v>
       </c>
       <c r="B555">
-        <v>6847054</v>
+        <v>6851957</v>
       </c>
       <c r="C555" t="s">
         <v>28</v>
@@ -49842,76 +49842,76 @@
         <v>45192.5</v>
       </c>
       <c r="F555" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G555" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H555">
+        <v>0</v>
+      </c>
+      <c r="I555">
         <v>1</v>
       </c>
-      <c r="I555">
-        <v>0</v>
-      </c>
       <c r="J555" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K555">
-        <v>1.95</v>
+        <v>1.181</v>
       </c>
       <c r="L555">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="M555">
-        <v>3.75</v>
+        <v>12</v>
       </c>
       <c r="N555">
-        <v>1.65</v>
+        <v>1.25</v>
       </c>
       <c r="O555">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="P555">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="Q555">
-        <v>-0.75</v>
+        <v>-1.75</v>
       </c>
       <c r="R555">
-        <v>1.85</v>
+        <v>1.925</v>
       </c>
       <c r="S555">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="T555">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U555">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V555">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W555">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X555">
         <v>-1</v>
       </c>
       <c r="Y555">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="Z555">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AA555">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="AB555">
         <v>-1</v>
       </c>
       <c r="AC555">
-        <v>0.8999999999999999</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="556" spans="1:29">
@@ -50720,7 +50720,7 @@
         <v>563</v>
       </c>
       <c r="B565">
-        <v>6847065</v>
+        <v>6851955</v>
       </c>
       <c r="C565" t="s">
         <v>28</v>
@@ -50732,13 +50732,13 @@
         <v>45206.5</v>
       </c>
       <c r="F565" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G565" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H565">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I565">
         <v>0</v>
@@ -50747,43 +50747,43 @@
         <v>45</v>
       </c>
       <c r="K565">
-        <v>1.8</v>
+        <v>1.727</v>
       </c>
       <c r="L565">
+        <v>3.75</v>
+      </c>
+      <c r="M565">
+        <v>4.5</v>
+      </c>
+      <c r="N565">
+        <v>1.909</v>
+      </c>
+      <c r="O565">
         <v>3.6</v>
       </c>
-      <c r="M565">
-        <v>4.333</v>
-      </c>
-      <c r="N565">
-        <v>1.571</v>
-      </c>
-      <c r="O565">
-        <v>4.333</v>
-      </c>
       <c r="P565">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="Q565">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="R565">
+        <v>1.9</v>
+      </c>
+      <c r="S565">
         <v>1.95</v>
       </c>
-      <c r="S565">
-        <v>1.9</v>
-      </c>
       <c r="T565">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U565">
-        <v>2</v>
+        <v>1.825</v>
       </c>
       <c r="V565">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="W565">
-        <v>0.571</v>
+        <v>0.909</v>
       </c>
       <c r="X565">
         <v>-1</v>
@@ -50792,16 +50792,16 @@
         <v>-1</v>
       </c>
       <c r="Z565">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA565">
         <v>-1</v>
       </c>
       <c r="AB565">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="AC565">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="566" spans="1:29">
@@ -50809,7 +50809,7 @@
         <v>564</v>
       </c>
       <c r="B566">
-        <v>6847064</v>
+        <v>6847065</v>
       </c>
       <c r="C566" t="s">
         <v>28</v>
@@ -50821,76 +50821,76 @@
         <v>45206.5</v>
       </c>
       <c r="F566" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G566" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H566">
+        <v>3</v>
+      </c>
+      <c r="I566">
         <v>0</v>
       </c>
-      <c r="I566">
-        <v>5</v>
-      </c>
       <c r="J566" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K566">
+        <v>1.8</v>
+      </c>
+      <c r="L566">
+        <v>3.6</v>
+      </c>
+      <c r="M566">
+        <v>4.333</v>
+      </c>
+      <c r="N566">
+        <v>1.571</v>
+      </c>
+      <c r="O566">
+        <v>4.333</v>
+      </c>
+      <c r="P566">
         <v>5.5</v>
       </c>
-      <c r="L566">
-        <v>4</v>
-      </c>
-      <c r="M566">
-        <v>1.571</v>
-      </c>
-      <c r="N566">
-        <v>7</v>
-      </c>
-      <c r="O566">
-        <v>5</v>
-      </c>
-      <c r="P566">
-        <v>1.4</v>
-      </c>
       <c r="Q566">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="R566">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="S566">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T566">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U566">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="V566">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="W566">
-        <v>-1</v>
+        <v>0.571</v>
       </c>
       <c r="X566">
         <v>-1</v>
       </c>
       <c r="Y566">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z566">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA566">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB566">
-        <v>1.025</v>
+        <v>0</v>
       </c>
       <c r="AC566">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="567" spans="1:29">
@@ -50898,7 +50898,7 @@
         <v>565</v>
       </c>
       <c r="B567">
-        <v>6851955</v>
+        <v>6847064</v>
       </c>
       <c r="C567" t="s">
         <v>28</v>
@@ -50910,73 +50910,73 @@
         <v>45206.5</v>
       </c>
       <c r="F567" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G567" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H567">
+        <v>0</v>
+      </c>
+      <c r="I567">
+        <v>5</v>
+      </c>
+      <c r="J567" t="s">
+        <v>46</v>
+      </c>
+      <c r="K567">
+        <v>5.5</v>
+      </c>
+      <c r="L567">
         <v>4</v>
       </c>
-      <c r="I567">
-        <v>0</v>
-      </c>
-      <c r="J567" t="s">
-        <v>45</v>
-      </c>
-      <c r="K567">
-        <v>1.727</v>
-      </c>
-      <c r="L567">
-        <v>3.75</v>
-      </c>
       <c r="M567">
-        <v>4.5</v>
+        <v>1.571</v>
       </c>
       <c r="N567">
-        <v>1.909</v>
+        <v>7</v>
       </c>
       <c r="O567">
-        <v>3.6</v>
+        <v>5</v>
       </c>
       <c r="P567">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="Q567">
-        <v>-0.5</v>
+        <v>1.25</v>
       </c>
       <c r="R567">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S567">
-        <v>1.95</v>
+        <v>1.875</v>
       </c>
       <c r="T567">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="U567">
+        <v>2.025</v>
+      </c>
+      <c r="V567">
         <v>1.825</v>
       </c>
-      <c r="V567">
-        <v>2.025</v>
-      </c>
       <c r="W567">
-        <v>0.909</v>
+        <v>-1</v>
       </c>
       <c r="X567">
         <v>-1</v>
       </c>
       <c r="Y567">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z567">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA567">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB567">
-        <v>0.825</v>
+        <v>1.025</v>
       </c>
       <c r="AC567">
         <v>-1</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 2024-02-03 às 11:02
</commit_message>
<xml_diff>
--- a/Austria Bundesliga/Austria Bundesliga.xlsx
+++ b/Austria Bundesliga/Austria Bundesliga.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -112,10 +112,10 @@
     <t>FC Salzburg</t>
   </si>
   <si>
-    <t>SCR Altach</t>
+    <t>SV Ried</t>
   </si>
   <si>
-    <t>SV Ried</t>
+    <t>SCR Altach</t>
   </si>
   <si>
     <t>FK Austria Vienna</t>
@@ -510,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC200"/>
+  <dimension ref="A1:AC202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -874,7 +874,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5205970</v>
+        <v>5205969</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -889,7 +889,7 @@
         <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -901,41 +901,41 @@
         <v>43</v>
       </c>
       <c r="K5">
-        <v>4.75</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>3.8</v>
+        <v>3.4</v>
       </c>
       <c r="M5">
-        <v>1.666</v>
+        <v>3.6</v>
       </c>
       <c r="N5">
-        <v>6</v>
+        <v>2.375</v>
       </c>
       <c r="O5">
-        <v>4.2</v>
+        <v>3.4</v>
       </c>
       <c r="P5">
-        <v>1.55</v>
+        <v>3</v>
       </c>
       <c r="Q5">
-        <v>1</v>
+        <v>-0.25</v>
       </c>
       <c r="R5">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S5">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="T5">
         <v>2.75</v>
       </c>
       <c r="U5">
+        <v>2.025</v>
+      </c>
+      <c r="V5">
         <v>1.825</v>
       </c>
-      <c r="V5">
-        <v>2.025</v>
-      </c>
       <c r="W5">
         <v>-1</v>
       </c>
@@ -943,19 +943,19 @@
         <v>-1</v>
       </c>
       <c r="Y5">
-        <v>0.55</v>
+        <v>2</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA5">
-        <v>-0</v>
+        <v>0.825</v>
       </c>
       <c r="AB5">
         <v>-1</v>
       </c>
       <c r="AC5">
-        <v>1.025</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -963,7 +963,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5205969</v>
+        <v>5205970</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -978,7 +978,7 @@
         <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -990,41 +990,41 @@
         <v>43</v>
       </c>
       <c r="K6">
-        <v>2</v>
+        <v>4.75</v>
       </c>
       <c r="L6">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="M6">
-        <v>3.6</v>
+        <v>1.666</v>
       </c>
       <c r="N6">
-        <v>2.375</v>
+        <v>6</v>
       </c>
       <c r="O6">
-        <v>3.4</v>
+        <v>4.2</v>
       </c>
       <c r="P6">
-        <v>3</v>
+        <v>1.55</v>
       </c>
       <c r="Q6">
-        <v>-0.25</v>
+        <v>1</v>
       </c>
       <c r="R6">
-        <v>2.025</v>
+        <v>1.95</v>
       </c>
       <c r="S6">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="T6">
         <v>2.75</v>
       </c>
       <c r="U6">
+        <v>1.825</v>
+      </c>
+      <c r="V6">
         <v>2.025</v>
       </c>
-      <c r="V6">
-        <v>1.825</v>
-      </c>
       <c r="W6">
         <v>-1</v>
       </c>
@@ -1032,19 +1032,19 @@
         <v>-1</v>
       </c>
       <c r="Y6">
-        <v>2</v>
+        <v>0.55</v>
       </c>
       <c r="Z6">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>0.825</v>
+        <v>-0</v>
       </c>
       <c r="AB6">
         <v>-1</v>
       </c>
       <c r="AC6">
-        <v>0.825</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -1242,7 +1242,7 @@
         <v>44975.54166666666</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
         <v>40</v>
@@ -1601,7 +1601,7 @@
         <v>39</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13">
         <v>3</v>
@@ -1954,7 +1954,7 @@
         <v>44983.4375</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G17" t="s">
         <v>38</v>
@@ -2135,7 +2135,7 @@
         <v>31</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H19">
         <v>2</v>
@@ -2399,7 +2399,7 @@
         <v>44989.54166666666</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
         <v>34</v>
@@ -2580,7 +2580,7 @@
         <v>36</v>
       </c>
       <c r="G24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H24">
         <v>3</v>
@@ -2743,7 +2743,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>5205987</v>
+        <v>5205988</v>
       </c>
       <c r="C26" t="s">
         <v>28</v>
@@ -2755,58 +2755,58 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" t="s">
         <v>42</v>
       </c>
       <c r="K26">
-        <v>1.7</v>
+        <v>1.909</v>
       </c>
       <c r="L26">
+        <v>3.6</v>
+      </c>
+      <c r="M26">
         <v>3.8</v>
       </c>
-      <c r="M26">
-        <v>4.75</v>
-      </c>
       <c r="N26">
-        <v>1.75</v>
+        <v>2.15</v>
       </c>
       <c r="O26">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="P26">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="Q26">
-        <v>-0.75</v>
+        <v>-0.25</v>
       </c>
       <c r="R26">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="S26">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="T26">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="U26">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V26">
-        <v>1.925</v>
+        <v>1.85</v>
       </c>
       <c r="W26">
-        <v>0.75</v>
+        <v>1.15</v>
       </c>
       <c r="X26">
         <v>-1</v>
@@ -2815,16 +2815,16 @@
         <v>-1</v>
       </c>
       <c r="Z26">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA26">
         <v>-1</v>
       </c>
       <c r="AB26">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AC26">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:29">
@@ -2832,7 +2832,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>5205988</v>
+        <v>5205989</v>
       </c>
       <c r="C27" t="s">
         <v>28</v>
@@ -2844,13 +2844,13 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F27" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2859,43 +2859,43 @@
         <v>42</v>
       </c>
       <c r="K27">
-        <v>1.909</v>
+        <v>1.6</v>
       </c>
       <c r="L27">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M27">
-        <v>3.8</v>
+        <v>5.25</v>
       </c>
       <c r="N27">
-        <v>2.15</v>
+        <v>1.6</v>
       </c>
       <c r="O27">
-        <v>3.4</v>
+        <v>4</v>
       </c>
       <c r="P27">
-        <v>3.3</v>
+        <v>5.75</v>
       </c>
       <c r="Q27">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="R27">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="S27">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="T27">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U27">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V27">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W27">
-        <v>1.15</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="X27">
         <v>-1</v>
@@ -2904,7 +2904,7 @@
         <v>-1</v>
       </c>
       <c r="Z27">
-        <v>0.8500000000000001</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA27">
         <v>-1</v>
@@ -2913,7 +2913,7 @@
         <v>-1</v>
       </c>
       <c r="AC27">
-        <v>0.8500000000000001</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="28" spans="1:29">
@@ -2921,7 +2921,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>5205989</v>
+        <v>5205990</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -2933,76 +2933,76 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K28">
-        <v>1.6</v>
+        <v>2.375</v>
       </c>
       <c r="L28">
-        <v>4</v>
+        <v>3.25</v>
       </c>
       <c r="M28">
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="N28">
-        <v>1.6</v>
+        <v>2.4</v>
       </c>
       <c r="O28">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="P28">
-        <v>5.75</v>
+        <v>3</v>
       </c>
       <c r="Q28">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="R28">
+        <v>2.1</v>
+      </c>
+      <c r="S28">
+        <v>1.775</v>
+      </c>
+      <c r="T28">
+        <v>2.5</v>
+      </c>
+      <c r="U28">
         <v>1.975</v>
       </c>
-      <c r="S28">
+      <c r="V28">
         <v>1.875</v>
       </c>
-      <c r="T28">
-        <v>3</v>
-      </c>
-      <c r="U28">
-        <v>2.025</v>
-      </c>
-      <c r="V28">
-        <v>1.825</v>
-      </c>
       <c r="W28">
-        <v>0.6000000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X28">
         <v>-1</v>
       </c>
       <c r="Y28">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="Z28">
+        <v>-1</v>
+      </c>
+      <c r="AA28">
+        <v>0.7749999999999999</v>
+      </c>
+      <c r="AB28">
         <v>0.9750000000000001</v>
       </c>
-      <c r="AA28">
-        <v>-1</v>
-      </c>
-      <c r="AB28">
-        <v>-1</v>
-      </c>
       <c r="AC28">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="29" spans="1:29">
@@ -3010,7 +3010,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>5205990</v>
+        <v>5205987</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -3022,73 +3022,73 @@
         <v>44997.54166666666</v>
       </c>
       <c r="F29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H29">
+        <v>3</v>
+      </c>
+      <c r="I29">
         <v>1</v>
       </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
       <c r="J29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K29">
-        <v>2.375</v>
+        <v>1.7</v>
       </c>
       <c r="L29">
-        <v>3.25</v>
+        <v>3.8</v>
       </c>
       <c r="M29">
-        <v>3</v>
+        <v>4.75</v>
       </c>
       <c r="N29">
-        <v>2.4</v>
+        <v>1.75</v>
       </c>
       <c r="O29">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
       <c r="P29">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="Q29">
-        <v>-0.25</v>
+        <v>-0.75</v>
       </c>
       <c r="R29">
-        <v>2.1</v>
+        <v>1.95</v>
       </c>
       <c r="S29">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="T29">
         <v>2.5</v>
       </c>
       <c r="U29">
-        <v>1.975</v>
+        <v>1.925</v>
       </c>
       <c r="V29">
-        <v>1.875</v>
+        <v>1.925</v>
       </c>
       <c r="W29">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="X29">
         <v>-1</v>
       </c>
       <c r="Y29">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="Z29">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA29">
-        <v>0.7749999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AB29">
-        <v>0.9750000000000001</v>
+        <v>0.925</v>
       </c>
       <c r="AC29">
         <v>-1</v>
@@ -3378,7 +3378,7 @@
         <v>45004.54166666666</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G33" t="s">
         <v>30</v>
@@ -3648,7 +3648,7 @@
         <v>31</v>
       </c>
       <c r="G36" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -3912,7 +3912,7 @@
         <v>45017.5</v>
       </c>
       <c r="F39" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G39" t="s">
         <v>38</v>
@@ -4004,7 +4004,7 @@
         <v>30</v>
       </c>
       <c r="G40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -4449,7 +4449,7 @@
         <v>37</v>
       </c>
       <c r="G45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H45">
         <v>1</v>
@@ -4535,7 +4535,7 @@
         <v>45024.5</v>
       </c>
       <c r="F46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G46" t="s">
         <v>35</v>
@@ -4891,7 +4891,7 @@
         <v>45030.60416666666</v>
       </c>
       <c r="F50" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G50" t="s">
         <v>38</v>
@@ -5072,7 +5072,7 @@
         <v>35</v>
       </c>
       <c r="G52" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H52">
         <v>2</v>
@@ -5146,7 +5146,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>6429782</v>
+        <v>6430233</v>
       </c>
       <c r="C53" t="s">
         <v>28</v>
@@ -5158,76 +5158,76 @@
         <v>45032.39583333334</v>
       </c>
       <c r="F53" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G53" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J53" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K53">
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="L53">
+        <v>3.8</v>
+      </c>
+      <c r="M53">
+        <v>1.65</v>
+      </c>
+      <c r="N53">
+        <v>7.5</v>
+      </c>
+      <c r="O53">
         <v>4.333</v>
       </c>
-      <c r="M53">
-        <v>6</v>
-      </c>
-      <c r="N53">
-        <v>1.5</v>
-      </c>
-      <c r="O53">
-        <v>4.5</v>
-      </c>
       <c r="P53">
-        <v>6</v>
+        <v>1.444</v>
       </c>
       <c r="Q53">
-        <v>-1.25</v>
+        <v>1.25</v>
       </c>
       <c r="R53">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="S53">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="T53">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U53">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="V53">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="W53">
         <v>-1</v>
       </c>
       <c r="X53">
-        <v>3.5</v>
+        <v>-1</v>
       </c>
       <c r="Y53">
-        <v>-1</v>
+        <v>0.444</v>
       </c>
       <c r="Z53">
         <v>-1</v>
       </c>
       <c r="AA53">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AB53">
         <v>-1</v>
       </c>
       <c r="AC53">
-        <v>0.875</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="54" spans="1:29">
@@ -5235,7 +5235,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>6430233</v>
+        <v>6429782</v>
       </c>
       <c r="C54" t="s">
         <v>28</v>
@@ -5247,76 +5247,76 @@
         <v>45032.39583333334</v>
       </c>
       <c r="F54" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G54" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J54" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K54">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="L54">
-        <v>3.8</v>
+        <v>4.333</v>
       </c>
       <c r="M54">
-        <v>1.65</v>
+        <v>6</v>
       </c>
       <c r="N54">
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="O54">
-        <v>4.333</v>
+        <v>4.5</v>
       </c>
       <c r="P54">
-        <v>1.444</v>
+        <v>6</v>
       </c>
       <c r="Q54">
-        <v>1.25</v>
+        <v>-1.25</v>
       </c>
       <c r="R54">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S54">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="T54">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U54">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="V54">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="W54">
         <v>-1</v>
       </c>
       <c r="X54">
-        <v>-1</v>
+        <v>3.5</v>
       </c>
       <c r="Y54">
-        <v>0.444</v>
+        <v>-1</v>
       </c>
       <c r="Z54">
         <v>-1</v>
       </c>
       <c r="AA54">
-        <v>0.95</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB54">
         <v>-1</v>
       </c>
       <c r="AC54">
-        <v>1.025</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="55" spans="1:29">
@@ -5502,7 +5502,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>6430211</v>
+        <v>6430210</v>
       </c>
       <c r="C57" t="s">
         <v>28</v>
@@ -5514,76 +5514,76 @@
         <v>45038.5</v>
       </c>
       <c r="F57" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G57" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
+        <v>44</v>
+      </c>
+      <c r="K57">
+        <v>2.55</v>
+      </c>
+      <c r="L57">
+        <v>3.3</v>
+      </c>
+      <c r="M57">
+        <v>2.7</v>
+      </c>
+      <c r="N57">
+        <v>2.5</v>
+      </c>
+      <c r="O57">
+        <v>3.3</v>
+      </c>
+      <c r="P57">
+        <v>2.875</v>
+      </c>
+      <c r="Q57">
         <v>0</v>
       </c>
-      <c r="I57">
-        <v>2</v>
-      </c>
-      <c r="J57" t="s">
-        <v>43</v>
-      </c>
-      <c r="K57">
-        <v>1.8</v>
-      </c>
-      <c r="L57">
-        <v>3.75</v>
-      </c>
-      <c r="M57">
-        <v>4.2</v>
-      </c>
-      <c r="N57">
-        <v>1.833</v>
-      </c>
-      <c r="O57">
-        <v>3.8</v>
-      </c>
-      <c r="P57">
-        <v>4</v>
-      </c>
-      <c r="Q57">
+      <c r="R57">
+        <v>1.825</v>
+      </c>
+      <c r="S57">
+        <v>2.025</v>
+      </c>
+      <c r="T57">
+        <v>2.25</v>
+      </c>
+      <c r="U57">
+        <v>1.85</v>
+      </c>
+      <c r="V57">
+        <v>2</v>
+      </c>
+      <c r="W57">
+        <v>-1</v>
+      </c>
+      <c r="X57">
+        <v>2.3</v>
+      </c>
+      <c r="Y57">
+        <v>-1</v>
+      </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
+      <c r="AA57">
+        <v>-0</v>
+      </c>
+      <c r="AB57">
         <v>-0.5</v>
       </c>
-      <c r="R57">
-        <v>1.85</v>
-      </c>
-      <c r="S57">
-        <v>2</v>
-      </c>
-      <c r="T57">
-        <v>2.75</v>
-      </c>
-      <c r="U57">
-        <v>1.925</v>
-      </c>
-      <c r="V57">
-        <v>1.925</v>
-      </c>
-      <c r="W57">
-        <v>-1</v>
-      </c>
-      <c r="X57">
-        <v>-1</v>
-      </c>
-      <c r="Y57">
-        <v>3</v>
-      </c>
-      <c r="Z57">
-        <v>-1</v>
-      </c>
-      <c r="AA57">
-        <v>1</v>
-      </c>
-      <c r="AB57">
-        <v>-1</v>
-      </c>
       <c r="AC57">
-        <v>0.925</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="58" spans="1:29">
@@ -5591,7 +5591,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>6430210</v>
+        <v>6430211</v>
       </c>
       <c r="C58" t="s">
         <v>28</v>
@@ -5603,76 +5603,76 @@
         <v>45038.5</v>
       </c>
       <c r="F58" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G58" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58" t="s">
+        <v>43</v>
+      </c>
+      <c r="K58">
+        <v>1.8</v>
+      </c>
+      <c r="L58">
+        <v>3.75</v>
+      </c>
+      <c r="M58">
+        <v>4.2</v>
+      </c>
+      <c r="N58">
+        <v>1.833</v>
+      </c>
+      <c r="O58">
+        <v>3.8</v>
+      </c>
+      <c r="P58">
+        <v>4</v>
+      </c>
+      <c r="Q58">
+        <v>-0.5</v>
+      </c>
+      <c r="R58">
+        <v>1.85</v>
+      </c>
+      <c r="S58">
+        <v>2</v>
+      </c>
+      <c r="T58">
+        <v>2.75</v>
+      </c>
+      <c r="U58">
+        <v>1.925</v>
+      </c>
+      <c r="V58">
+        <v>1.925</v>
+      </c>
+      <c r="W58">
+        <v>-1</v>
+      </c>
+      <c r="X58">
+        <v>-1</v>
+      </c>
+      <c r="Y58">
+        <v>3</v>
+      </c>
+      <c r="Z58">
+        <v>-1</v>
+      </c>
+      <c r="AA58">
         <v>1</v>
       </c>
-      <c r="I58">
-        <v>1</v>
-      </c>
-      <c r="J58" t="s">
-        <v>44</v>
-      </c>
-      <c r="K58">
-        <v>2.55</v>
-      </c>
-      <c r="L58">
-        <v>3.3</v>
-      </c>
-      <c r="M58">
-        <v>2.7</v>
-      </c>
-      <c r="N58">
-        <v>2.5</v>
-      </c>
-      <c r="O58">
-        <v>3.3</v>
-      </c>
-      <c r="P58">
-        <v>2.875</v>
-      </c>
-      <c r="Q58">
-        <v>0</v>
-      </c>
-      <c r="R58">
-        <v>1.825</v>
-      </c>
-      <c r="S58">
-        <v>2.025</v>
-      </c>
-      <c r="T58">
-        <v>2.25</v>
-      </c>
-      <c r="U58">
-        <v>1.85</v>
-      </c>
-      <c r="V58">
-        <v>2</v>
-      </c>
-      <c r="W58">
-        <v>-1</v>
-      </c>
-      <c r="X58">
-        <v>2.3</v>
-      </c>
-      <c r="Y58">
-        <v>-1</v>
-      </c>
-      <c r="Z58">
-        <v>0</v>
-      </c>
-      <c r="AA58">
-        <v>-0</v>
-      </c>
       <c r="AB58">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="AC58">
-        <v>0.5</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="59" spans="1:29">
@@ -6137,7 +6137,7 @@
         <v>45044.60416666666</v>
       </c>
       <c r="F64" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G64" t="s">
         <v>30</v>
@@ -6226,7 +6226,7 @@
         <v>45045.5</v>
       </c>
       <c r="F65" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G65" t="s">
         <v>37</v>
@@ -6496,7 +6496,7 @@
         <v>30</v>
       </c>
       <c r="G68" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -6585,7 +6585,7 @@
         <v>37</v>
       </c>
       <c r="G69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H69">
         <v>2</v>
@@ -7030,7 +7030,7 @@
         <v>38</v>
       </c>
       <c r="G74" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H74">
         <v>1</v>
@@ -7205,7 +7205,7 @@
         <v>45059.5</v>
       </c>
       <c r="F76" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G76" t="s">
         <v>35</v>
@@ -7561,10 +7561,10 @@
         <v>45065.60416666666</v>
       </c>
       <c r="F80" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" t="s">
         <v>33</v>
-      </c>
-      <c r="G80" t="s">
-        <v>32</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -7638,7 +7638,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6430223</v>
+        <v>6430222</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
@@ -7650,55 +7650,55 @@
         <v>45066.5</v>
       </c>
       <c r="F81" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G81" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I81">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J81" t="s">
         <v>43</v>
       </c>
       <c r="K81">
-        <v>2.45</v>
+        <v>2.2</v>
       </c>
       <c r="L81">
         <v>3.4</v>
       </c>
       <c r="M81">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="N81">
-        <v>2.9</v>
+        <v>1.95</v>
       </c>
       <c r="O81">
-        <v>3.4</v>
+        <v>3.75</v>
       </c>
       <c r="P81">
-        <v>2.375</v>
+        <v>3.75</v>
       </c>
       <c r="Q81">
-        <v>0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R81">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="S81">
-        <v>2.05</v>
+        <v>1.95</v>
       </c>
       <c r="T81">
         <v>2.75</v>
       </c>
       <c r="U81">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="V81">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="W81">
         <v>-1</v>
@@ -7707,19 +7707,19 @@
         <v>-1</v>
       </c>
       <c r="Y81">
-        <v>1.375</v>
+        <v>2.75</v>
       </c>
       <c r="Z81">
         <v>-1</v>
       </c>
       <c r="AA81">
-        <v>1.05</v>
+        <v>0.95</v>
       </c>
       <c r="AB81">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC81">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
     </row>
     <row r="82" spans="1:29">
@@ -7727,7 +7727,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6430222</v>
+        <v>6430223</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
@@ -7739,55 +7739,55 @@
         <v>45066.5</v>
       </c>
       <c r="F82" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G82" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I82">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J82" t="s">
         <v>43</v>
       </c>
       <c r="K82">
-        <v>2.2</v>
+        <v>2.45</v>
       </c>
       <c r="L82">
         <v>3.4</v>
       </c>
       <c r="M82">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="N82">
-        <v>1.95</v>
+        <v>2.9</v>
       </c>
       <c r="O82">
-        <v>3.75</v>
+        <v>3.4</v>
       </c>
       <c r="P82">
-        <v>3.75</v>
+        <v>2.375</v>
       </c>
       <c r="Q82">
-        <v>-0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R82">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="S82">
-        <v>1.95</v>
+        <v>2.05</v>
       </c>
       <c r="T82">
         <v>2.75</v>
       </c>
       <c r="U82">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="V82">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="W82">
         <v>-1</v>
@@ -7796,19 +7796,19 @@
         <v>-1</v>
       </c>
       <c r="Y82">
-        <v>2.75</v>
+        <v>1.375</v>
       </c>
       <c r="Z82">
         <v>-1</v>
       </c>
       <c r="AA82">
-        <v>0.95</v>
+        <v>1.05</v>
       </c>
       <c r="AB82">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC82">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="83" spans="1:29">
@@ -7816,7 +7816,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>6429905</v>
+        <v>6430238</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
@@ -7828,10 +7828,10 @@
         <v>45067.39583333334</v>
       </c>
       <c r="F83" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G83" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -7843,61 +7843,61 @@
         <v>44</v>
       </c>
       <c r="K83">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="L83">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="M83">
-        <v>1.909</v>
+        <v>2.7</v>
       </c>
       <c r="N83">
-        <v>5</v>
+        <v>2.7</v>
       </c>
       <c r="O83">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="P83">
-        <v>1.571</v>
+        <v>2.55</v>
       </c>
       <c r="Q83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R83">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="S83">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="T83">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U83">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V83">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W83">
         <v>-1</v>
       </c>
       <c r="X83">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="Y83">
         <v>-1</v>
       </c>
       <c r="Z83">
-        <v>0.8999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AA83">
-        <v>-1</v>
+        <v>-0</v>
       </c>
       <c r="AB83">
         <v>-1</v>
       </c>
       <c r="AC83">
-        <v>0.825</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="84" spans="1:29">
@@ -7905,7 +7905,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>6430238</v>
+        <v>6429905</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
@@ -7917,10 +7917,10 @@
         <v>45067.39583333334</v>
       </c>
       <c r="F84" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G84" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -7932,61 +7932,61 @@
         <v>44</v>
       </c>
       <c r="K84">
-        <v>2.5</v>
+        <v>3.75</v>
       </c>
       <c r="L84">
-        <v>3.4</v>
+        <v>3.6</v>
       </c>
       <c r="M84">
-        <v>2.7</v>
+        <v>1.909</v>
       </c>
       <c r="N84">
-        <v>2.7</v>
+        <v>5</v>
       </c>
       <c r="O84">
+        <v>4.5</v>
+      </c>
+      <c r="P84">
+        <v>1.571</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+      <c r="R84">
+        <v>1.9</v>
+      </c>
+      <c r="S84">
+        <v>1.95</v>
+      </c>
+      <c r="T84">
+        <v>3.25</v>
+      </c>
+      <c r="U84">
+        <v>2.025</v>
+      </c>
+      <c r="V84">
+        <v>1.825</v>
+      </c>
+      <c r="W84">
+        <v>-1</v>
+      </c>
+      <c r="X84">
         <v>3.5</v>
       </c>
-      <c r="P84">
-        <v>2.55</v>
-      </c>
-      <c r="Q84">
-        <v>0</v>
-      </c>
-      <c r="R84">
-        <v>2</v>
-      </c>
-      <c r="S84">
-        <v>1.85</v>
-      </c>
-      <c r="T84">
-        <v>3</v>
-      </c>
-      <c r="U84">
-        <v>1.975</v>
-      </c>
-      <c r="V84">
-        <v>1.875</v>
-      </c>
-      <c r="W84">
-        <v>-1</v>
-      </c>
-      <c r="X84">
-        <v>2.5</v>
-      </c>
       <c r="Y84">
         <v>-1</v>
       </c>
       <c r="Z84">
-        <v>0</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA84">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB84">
         <v>-1</v>
       </c>
       <c r="AC84">
-        <v>0.875</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="85" spans="1:29">
@@ -8098,7 +8098,7 @@
         <v>35</v>
       </c>
       <c r="G86" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H86">
         <v>2</v>
@@ -8273,7 +8273,7 @@
         <v>45073.5</v>
       </c>
       <c r="F88" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G88" t="s">
         <v>37</v>
@@ -8617,7 +8617,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>6430227</v>
+        <v>6430228</v>
       </c>
       <c r="C92" t="s">
         <v>28</v>
@@ -8629,76 +8629,76 @@
         <v>45079.60416666666</v>
       </c>
       <c r="F92" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G92" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H92">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I92">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J92" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K92">
-        <v>2.625</v>
+        <v>2.55</v>
       </c>
       <c r="L92">
         <v>3.4</v>
       </c>
       <c r="M92">
-        <v>2.55</v>
+        <v>2.625</v>
       </c>
       <c r="N92">
-        <v>3.75</v>
+        <v>2.8</v>
       </c>
       <c r="O92">
-        <v>3.6</v>
+        <v>3.8</v>
       </c>
       <c r="P92">
-        <v>1.95</v>
+        <v>2.3</v>
       </c>
       <c r="Q92">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="R92">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="S92">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="T92">
         <v>2.75</v>
       </c>
       <c r="U92">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V92">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W92">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="X92">
         <v>-1</v>
       </c>
       <c r="Y92">
-        <v>-1</v>
+        <v>1.3</v>
       </c>
       <c r="Z92">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA92">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="AB92">
-        <v>0.8999999999999999</v>
+        <v>0.4625</v>
       </c>
       <c r="AC92">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="93" spans="1:29">
@@ -8706,7 +8706,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>6430228</v>
+        <v>6430227</v>
       </c>
       <c r="C93" t="s">
         <v>28</v>
@@ -8718,76 +8718,76 @@
         <v>45079.60416666666</v>
       </c>
       <c r="F93" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G93" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H93">
+        <v>5</v>
+      </c>
+      <c r="I93">
         <v>1</v>
       </c>
-      <c r="I93">
-        <v>2</v>
-      </c>
       <c r="J93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K93">
-        <v>2.55</v>
+        <v>2.625</v>
       </c>
       <c r="L93">
         <v>3.4</v>
       </c>
       <c r="M93">
-        <v>2.625</v>
+        <v>2.55</v>
       </c>
       <c r="N93">
-        <v>2.8</v>
+        <v>3.75</v>
       </c>
       <c r="O93">
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="P93">
-        <v>2.3</v>
+        <v>1.95</v>
       </c>
       <c r="Q93">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="R93">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="S93">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="T93">
         <v>2.75</v>
       </c>
       <c r="U93">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="V93">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="W93">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="X93">
         <v>-1</v>
       </c>
       <c r="Y93">
-        <v>1.3</v>
+        <v>-1</v>
       </c>
       <c r="Z93">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AA93">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB93">
-        <v>0.4625</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC93">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="94" spans="1:29">
@@ -8810,7 +8810,7 @@
         <v>38</v>
       </c>
       <c r="G94" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H94">
         <v>1</v>
@@ -9329,7 +9329,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>6847027</v>
+        <v>6847026</v>
       </c>
       <c r="C100" t="s">
         <v>28</v>
@@ -9341,73 +9341,73 @@
         <v>45136.5</v>
       </c>
       <c r="F100" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G100" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J100" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K100">
         <v>2.1</v>
       </c>
       <c r="L100">
-        <v>3.4</v>
+        <v>3.25</v>
       </c>
       <c r="M100">
-        <v>3.1</v>
+        <v>3.25</v>
       </c>
       <c r="N100">
-        <v>2.3</v>
+        <v>1.833</v>
       </c>
       <c r="O100">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="P100">
-        <v>2.8</v>
+        <v>4.2</v>
       </c>
       <c r="Q100">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R100">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="S100">
-        <v>1.825</v>
+        <v>1.975</v>
       </c>
       <c r="T100">
         <v>2.75</v>
       </c>
       <c r="U100">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="V100">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="W100">
         <v>-1</v>
       </c>
       <c r="X100">
-        <v>-1</v>
+        <v>2.75</v>
       </c>
       <c r="Y100">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="Z100">
         <v>-1</v>
       </c>
       <c r="AA100">
-        <v>0.825</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB100">
-        <v>0.825</v>
+        <v>0.925</v>
       </c>
       <c r="AC100">
         <v>-1</v>
@@ -9418,7 +9418,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>6847026</v>
+        <v>6847027</v>
       </c>
       <c r="C101" t="s">
         <v>28</v>
@@ -9430,73 +9430,73 @@
         <v>45136.5</v>
       </c>
       <c r="F101" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G101" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I101">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J101" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K101">
         <v>2.1</v>
       </c>
       <c r="L101">
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="M101">
-        <v>3.25</v>
+        <v>3.1</v>
       </c>
       <c r="N101">
-        <v>1.833</v>
+        <v>2.3</v>
       </c>
       <c r="O101">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="P101">
-        <v>4.2</v>
+        <v>2.8</v>
       </c>
       <c r="Q101">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R101">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="S101">
-        <v>1.975</v>
+        <v>1.825</v>
       </c>
       <c r="T101">
         <v>2.75</v>
       </c>
       <c r="U101">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="V101">
-        <v>1.925</v>
+        <v>2.025</v>
       </c>
       <c r="W101">
         <v>-1</v>
       </c>
       <c r="X101">
-        <v>2.75</v>
+        <v>-1</v>
       </c>
       <c r="Y101">
-        <v>-1</v>
+        <v>1.8</v>
       </c>
       <c r="Z101">
         <v>-1</v>
       </c>
       <c r="AA101">
-        <v>0.9750000000000001</v>
+        <v>0.825</v>
       </c>
       <c r="AB101">
-        <v>0.925</v>
+        <v>0.825</v>
       </c>
       <c r="AC101">
         <v>-1</v>
@@ -9519,7 +9519,7 @@
         <v>45136.60416666666</v>
       </c>
       <c r="F102" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G102" t="s">
         <v>31</v>
@@ -9700,7 +9700,7 @@
         <v>39</v>
       </c>
       <c r="G104" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H104">
         <v>4</v>
@@ -9863,7 +9863,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>6851963</v>
+        <v>6846459</v>
       </c>
       <c r="C106" t="s">
         <v>28</v>
@@ -9875,76 +9875,76 @@
         <v>45144.5</v>
       </c>
       <c r="F106" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G106" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H106">
         <v>3</v>
       </c>
       <c r="I106">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J106" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K106">
-        <v>2.7</v>
+        <v>1.142</v>
       </c>
       <c r="L106">
-        <v>3.4</v>
+        <v>8</v>
       </c>
       <c r="M106">
-        <v>2.55</v>
+        <v>17</v>
       </c>
       <c r="N106">
-        <v>2.25</v>
+        <v>1.166</v>
       </c>
       <c r="O106">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="P106">
-        <v>3.1</v>
+        <v>15</v>
       </c>
       <c r="Q106">
-        <v>-0.25</v>
+        <v>-2.25</v>
       </c>
       <c r="R106">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="S106">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="T106">
-        <v>2.75</v>
+        <v>3.75</v>
       </c>
       <c r="U106">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="V106">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="W106">
-        <v>-1</v>
+        <v>0.1659999999999999</v>
       </c>
       <c r="X106">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="Y106">
         <v>-1</v>
       </c>
       <c r="Z106">
-        <v>-0.5</v>
+        <v>0.95</v>
       </c>
       <c r="AA106">
-        <v>0.4375</v>
+        <v>-1</v>
       </c>
       <c r="AB106">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AC106">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="107" spans="1:29">
@@ -9952,7 +9952,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>6846459</v>
+        <v>6851963</v>
       </c>
       <c r="C107" t="s">
         <v>28</v>
@@ -9964,76 +9964,76 @@
         <v>45144.5</v>
       </c>
       <c r="F107" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G107" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H107">
         <v>3</v>
       </c>
       <c r="I107">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J107" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K107">
-        <v>1.142</v>
+        <v>2.7</v>
       </c>
       <c r="L107">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="M107">
-        <v>17</v>
+        <v>2.55</v>
       </c>
       <c r="N107">
-        <v>1.166</v>
+        <v>2.25</v>
       </c>
       <c r="O107">
-        <v>7.5</v>
+        <v>3.5</v>
       </c>
       <c r="P107">
-        <v>15</v>
+        <v>3.1</v>
       </c>
       <c r="Q107">
-        <v>-2.25</v>
+        <v>-0.25</v>
       </c>
       <c r="R107">
+        <v>1.975</v>
+      </c>
+      <c r="S107">
+        <v>1.875</v>
+      </c>
+      <c r="T107">
+        <v>2.75</v>
+      </c>
+      <c r="U107">
+        <v>1.9</v>
+      </c>
+      <c r="V107">
         <v>1.95</v>
       </c>
-      <c r="S107">
-        <v>1.9</v>
-      </c>
-      <c r="T107">
-        <v>3.75</v>
-      </c>
-      <c r="U107">
-        <v>1.925</v>
-      </c>
-      <c r="V107">
-        <v>1.925</v>
-      </c>
       <c r="W107">
-        <v>0.1659999999999999</v>
+        <v>-1</v>
       </c>
       <c r="X107">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="Y107">
         <v>-1</v>
       </c>
       <c r="Z107">
-        <v>0.95</v>
+        <v>-0.5</v>
       </c>
       <c r="AA107">
-        <v>-1</v>
+        <v>0.4375</v>
       </c>
       <c r="AB107">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AC107">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="108" spans="1:29">
@@ -10676,7 +10676,7 @@
         <v>45151.5</v>
       </c>
       <c r="F115" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G115" t="s">
         <v>38</v>
@@ -10946,7 +10946,7 @@
         <v>36</v>
       </c>
       <c r="G118" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H118">
         <v>1</v>
@@ -11480,7 +11480,7 @@
         <v>37</v>
       </c>
       <c r="G124" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -11554,7 +11554,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>6847044</v>
+        <v>6847043</v>
       </c>
       <c r="C125" t="s">
         <v>28</v>
@@ -11566,49 +11566,49 @@
         <v>45165.5</v>
       </c>
       <c r="F125" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G125" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J125" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K125">
-        <v>2.75</v>
+        <v>1.615</v>
       </c>
       <c r="L125">
+        <v>3.9</v>
+      </c>
+      <c r="M125">
+        <v>4.2</v>
+      </c>
+      <c r="N125">
+        <v>1.4</v>
+      </c>
+      <c r="O125">
+        <v>5.5</v>
+      </c>
+      <c r="P125">
+        <v>6</v>
+      </c>
+      <c r="Q125">
+        <v>-1.25</v>
+      </c>
+      <c r="R125">
+        <v>1.825</v>
+      </c>
+      <c r="S125">
+        <v>2.025</v>
+      </c>
+      <c r="T125">
         <v>3.25</v>
-      </c>
-      <c r="M125">
-        <v>2.25</v>
-      </c>
-      <c r="N125">
-        <v>2.1</v>
-      </c>
-      <c r="O125">
-        <v>3.5</v>
-      </c>
-      <c r="P125">
-        <v>3.3</v>
-      </c>
-      <c r="Q125">
-        <v>-0.25</v>
-      </c>
-      <c r="R125">
-        <v>1.8</v>
-      </c>
-      <c r="S125">
-        <v>2.05</v>
-      </c>
-      <c r="T125">
-        <v>2.5</v>
       </c>
       <c r="U125">
         <v>1.875</v>
@@ -11620,22 +11620,22 @@
         <v>-1</v>
       </c>
       <c r="X125">
-        <v>-1</v>
+        <v>4.5</v>
       </c>
       <c r="Y125">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="Z125">
         <v>-1</v>
       </c>
       <c r="AA125">
-        <v>1.05</v>
+        <v>1.025</v>
       </c>
       <c r="AB125">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AC125">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
     </row>
     <row r="126" spans="1:29">
@@ -11643,7 +11643,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>6847043</v>
+        <v>6847042</v>
       </c>
       <c r="C126" t="s">
         <v>28</v>
@@ -11655,76 +11655,76 @@
         <v>45165.5</v>
       </c>
       <c r="F126" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G126" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H126">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J126" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K126">
-        <v>1.615</v>
+        <v>1.909</v>
       </c>
       <c r="L126">
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="M126">
-        <v>4.2</v>
+        <v>3.25</v>
       </c>
       <c r="N126">
-        <v>1.4</v>
+        <v>1.85</v>
       </c>
       <c r="O126">
-        <v>5.5</v>
+        <v>3.8</v>
       </c>
       <c r="P126">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q126">
-        <v>-1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R126">
-        <v>1.825</v>
+        <v>1.85</v>
       </c>
       <c r="S126">
-        <v>2.025</v>
+        <v>2</v>
       </c>
       <c r="T126">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="U126">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="V126">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="W126">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="X126">
-        <v>4.5</v>
+        <v>-1</v>
       </c>
       <c r="Y126">
         <v>-1</v>
       </c>
       <c r="Z126">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AA126">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="AB126">
         <v>-1</v>
       </c>
       <c r="AC126">
-        <v>0.9750000000000001</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="127" spans="1:29">
@@ -11732,7 +11732,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>6847042</v>
+        <v>6847044</v>
       </c>
       <c r="C127" t="s">
         <v>28</v>
@@ -11744,76 +11744,76 @@
         <v>45165.5</v>
       </c>
       <c r="F127" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G127" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H127">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I127">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J127" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K127">
-        <v>1.909</v>
+        <v>2.75</v>
       </c>
       <c r="L127">
+        <v>3.25</v>
+      </c>
+      <c r="M127">
+        <v>2.25</v>
+      </c>
+      <c r="N127">
+        <v>2.1</v>
+      </c>
+      <c r="O127">
         <v>3.5</v>
       </c>
-      <c r="M127">
-        <v>3.25</v>
-      </c>
-      <c r="N127">
-        <v>1.85</v>
-      </c>
-      <c r="O127">
-        <v>3.8</v>
-      </c>
       <c r="P127">
-        <v>4</v>
+        <v>3.3</v>
       </c>
       <c r="Q127">
-        <v>-0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="R127">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S127">
-        <v>2</v>
+        <v>2.05</v>
       </c>
       <c r="T127">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="U127">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="V127">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="W127">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="X127">
         <v>-1</v>
       </c>
       <c r="Y127">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="Z127">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AA127">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="AB127">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AC127">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="128" spans="1:29">
@@ -12011,7 +12011,7 @@
         <v>45171.60416666666</v>
       </c>
       <c r="F130" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G130" t="s">
         <v>29</v>
@@ -12370,7 +12370,7 @@
         <v>41</v>
       </c>
       <c r="G134" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H134">
         <v>1</v>
@@ -13168,7 +13168,7 @@
         <v>45193.39583333334</v>
       </c>
       <c r="F143" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G143" t="s">
         <v>34</v>
@@ -13423,7 +13423,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>6851956</v>
+        <v>6847058</v>
       </c>
       <c r="C146" t="s">
         <v>28</v>
@@ -13435,76 +13435,76 @@
         <v>45199.5</v>
       </c>
       <c r="F146" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="G146" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J146" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K146">
-        <v>3</v>
+        <v>3.6</v>
       </c>
       <c r="L146">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
       <c r="M146">
-        <v>2.2</v>
+        <v>2</v>
       </c>
       <c r="N146">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
       <c r="O146">
         <v>3.4</v>
       </c>
       <c r="P146">
-        <v>2.625</v>
+        <v>2.25</v>
       </c>
       <c r="Q146">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R146">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="S146">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="T146">
         <v>2.5</v>
       </c>
       <c r="U146">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="V146">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="W146">
-        <v>-1</v>
+        <v>2.2</v>
       </c>
       <c r="X146">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="Y146">
         <v>-1</v>
       </c>
       <c r="Z146">
-        <v>0</v>
+        <v>0.875</v>
       </c>
       <c r="AA146">
-        <v>-0</v>
+        <v>-1</v>
       </c>
       <c r="AB146">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AC146">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="147" spans="1:29">
@@ -13512,7 +13512,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>6847058</v>
+        <v>6846465</v>
       </c>
       <c r="C147" t="s">
         <v>28</v>
@@ -13524,73 +13524,73 @@
         <v>45199.5</v>
       </c>
       <c r="F147" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G147" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I147">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J147" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K147">
-        <v>3.6</v>
+        <v>12</v>
       </c>
       <c r="L147">
+        <v>8</v>
+      </c>
+      <c r="M147">
+        <v>1.166</v>
+      </c>
+      <c r="N147">
+        <v>11</v>
+      </c>
+      <c r="O147">
+        <v>8</v>
+      </c>
+      <c r="P147">
+        <v>1.181</v>
+      </c>
+      <c r="Q147">
+        <v>2</v>
+      </c>
+      <c r="R147">
+        <v>2</v>
+      </c>
+      <c r="S147">
+        <v>1.85</v>
+      </c>
+      <c r="T147">
         <v>3.5</v>
       </c>
-      <c r="M147">
-        <v>2</v>
-      </c>
-      <c r="N147">
-        <v>3.2</v>
-      </c>
-      <c r="O147">
-        <v>3.4</v>
-      </c>
-      <c r="P147">
-        <v>2.25</v>
-      </c>
-      <c r="Q147">
-        <v>0.25</v>
-      </c>
-      <c r="R147">
-        <v>1.875</v>
-      </c>
-      <c r="S147">
-        <v>1.975</v>
-      </c>
-      <c r="T147">
-        <v>2.5</v>
-      </c>
       <c r="U147">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="V147">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="W147">
-        <v>2.2</v>
+        <v>-1</v>
       </c>
       <c r="X147">
         <v>-1</v>
       </c>
       <c r="Y147">
-        <v>-1</v>
+        <v>0.181</v>
       </c>
       <c r="Z147">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AA147">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB147">
-        <v>0.8500000000000001</v>
+        <v>0.95</v>
       </c>
       <c r="AC147">
         <v>-1</v>
@@ -13601,7 +13601,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>6846465</v>
+        <v>6851956</v>
       </c>
       <c r="C148" t="s">
         <v>28</v>
@@ -13613,76 +13613,76 @@
         <v>45199.5</v>
       </c>
       <c r="F148" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G148" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H148">
         <v>0</v>
       </c>
       <c r="I148">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J148" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K148">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="L148">
-        <v>8</v>
+        <v>3.6</v>
       </c>
       <c r="M148">
-        <v>1.166</v>
+        <v>2.2</v>
       </c>
       <c r="N148">
-        <v>11</v>
+        <v>2.6</v>
       </c>
       <c r="O148">
-        <v>8</v>
+        <v>3.4</v>
       </c>
       <c r="P148">
-        <v>1.181</v>
+        <v>2.625</v>
       </c>
       <c r="Q148">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R148">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="S148">
-        <v>1.85</v>
+        <v>1.95</v>
       </c>
       <c r="T148">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="U148">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="V148">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="W148">
         <v>-1</v>
       </c>
       <c r="X148">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="Y148">
-        <v>0.181</v>
+        <v>-1</v>
       </c>
       <c r="Z148">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA148">
-        <v>0.8500000000000001</v>
+        <v>-0</v>
       </c>
       <c r="AB148">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AC148">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="149" spans="1:29">
@@ -13794,7 +13794,7 @@
         <v>35</v>
       </c>
       <c r="G150" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -13957,7 +13957,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>6851955</v>
+        <v>6847065</v>
       </c>
       <c r="C152" t="s">
         <v>28</v>
@@ -13969,13 +13969,13 @@
         <v>45206.5</v>
       </c>
       <c r="F152" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G152" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H152">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I152">
         <v>0</v>
@@ -13984,43 +13984,43 @@
         <v>42</v>
       </c>
       <c r="K152">
-        <v>1.727</v>
+        <v>1.8</v>
       </c>
       <c r="L152">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="M152">
-        <v>4.5</v>
+        <v>4.333</v>
       </c>
       <c r="N152">
-        <v>1.909</v>
+        <v>1.571</v>
       </c>
       <c r="O152">
-        <v>3.6</v>
+        <v>4.333</v>
       </c>
       <c r="P152">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="Q152">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="R152">
+        <v>1.95</v>
+      </c>
+      <c r="S152">
         <v>1.9</v>
       </c>
-      <c r="S152">
-        <v>1.95</v>
-      </c>
       <c r="T152">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="U152">
-        <v>1.825</v>
+        <v>2</v>
       </c>
       <c r="V152">
-        <v>2.025</v>
+        <v>1.85</v>
       </c>
       <c r="W152">
-        <v>0.909</v>
+        <v>0.571</v>
       </c>
       <c r="X152">
         <v>-1</v>
@@ -14029,16 +14029,16 @@
         <v>-1</v>
       </c>
       <c r="Z152">
-        <v>0.8999999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AA152">
         <v>-1</v>
       </c>
       <c r="AB152">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="AC152">
-        <v>-1</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="153" spans="1:29">
@@ -14046,7 +14046,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>6847064</v>
+        <v>6851955</v>
       </c>
       <c r="C153" t="s">
         <v>28</v>
@@ -14058,73 +14058,73 @@
         <v>45206.5</v>
       </c>
       <c r="F153" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G153" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H153">
+        <v>4</v>
+      </c>
+      <c r="I153">
         <v>0</v>
       </c>
-      <c r="I153">
-        <v>5</v>
-      </c>
       <c r="J153" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K153">
-        <v>5.5</v>
+        <v>1.727</v>
       </c>
       <c r="L153">
+        <v>3.75</v>
+      </c>
+      <c r="M153">
+        <v>4.5</v>
+      </c>
+      <c r="N153">
+        <v>1.909</v>
+      </c>
+      <c r="O153">
+        <v>3.6</v>
+      </c>
+      <c r="P153">
         <v>4</v>
       </c>
-      <c r="M153">
-        <v>1.571</v>
-      </c>
-      <c r="N153">
-        <v>7</v>
-      </c>
-      <c r="O153">
-        <v>5</v>
-      </c>
-      <c r="P153">
-        <v>1.4</v>
-      </c>
       <c r="Q153">
-        <v>1.25</v>
+        <v>-0.5</v>
       </c>
       <c r="R153">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S153">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="T153">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="U153">
+        <v>1.825</v>
+      </c>
+      <c r="V153">
         <v>2.025</v>
       </c>
-      <c r="V153">
-        <v>1.825</v>
-      </c>
       <c r="W153">
-        <v>-1</v>
+        <v>0.909</v>
       </c>
       <c r="X153">
         <v>-1</v>
       </c>
       <c r="Y153">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="Z153">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA153">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB153">
-        <v>1.025</v>
+        <v>0.825</v>
       </c>
       <c r="AC153">
         <v>-1</v>
@@ -14135,7 +14135,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>6847065</v>
+        <v>6847064</v>
       </c>
       <c r="C154" t="s">
         <v>28</v>
@@ -14147,76 +14147,76 @@
         <v>45206.5</v>
       </c>
       <c r="F154" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G154" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H154">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I154">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J154" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K154">
-        <v>1.8</v>
+        <v>5.5</v>
       </c>
       <c r="L154">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="M154">
-        <v>4.333</v>
+        <v>1.571</v>
       </c>
       <c r="N154">
-        <v>1.571</v>
+        <v>7</v>
       </c>
       <c r="O154">
-        <v>4.333</v>
+        <v>5</v>
       </c>
       <c r="P154">
-        <v>5.5</v>
+        <v>1.4</v>
       </c>
       <c r="Q154">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="R154">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="S154">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="T154">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="U154">
-        <v>2</v>
+        <v>2.025</v>
       </c>
       <c r="V154">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="W154">
-        <v>0.571</v>
+        <v>-1</v>
       </c>
       <c r="X154">
         <v>-1</v>
       </c>
       <c r="Y154">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="Z154">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA154">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB154">
-        <v>0</v>
+        <v>1.025</v>
       </c>
       <c r="AC154">
-        <v>-0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="155" spans="1:29">
@@ -14328,7 +14328,7 @@
         <v>40</v>
       </c>
       <c r="G156" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H156">
         <v>1</v>
@@ -14770,7 +14770,7 @@
         <v>45221.39583333334</v>
       </c>
       <c r="F161" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G161" t="s">
         <v>30</v>
@@ -15040,7 +15040,7 @@
         <v>31</v>
       </c>
       <c r="G164" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H164">
         <v>3</v>
@@ -15838,7 +15838,7 @@
         <v>45235.4375</v>
       </c>
       <c r="F173" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G173" t="s">
         <v>39</v>
@@ -16108,7 +16108,7 @@
         <v>38</v>
       </c>
       <c r="G176" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H176">
         <v>5</v>
@@ -16182,7 +16182,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>6847079</v>
+        <v>6847080</v>
       </c>
       <c r="C177" t="s">
         <v>28</v>
@@ -16194,76 +16194,76 @@
         <v>45241.54166666666</v>
       </c>
       <c r="F177" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G177" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H177">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I177">
+        <v>0</v>
+      </c>
+      <c r="J177" t="s">
+        <v>42</v>
+      </c>
+      <c r="K177">
+        <v>3.2</v>
+      </c>
+      <c r="L177">
+        <v>3.5</v>
+      </c>
+      <c r="M177">
+        <v>2.15</v>
+      </c>
+      <c r="N177">
+        <v>3.5</v>
+      </c>
+      <c r="O177">
+        <v>3.75</v>
+      </c>
+      <c r="P177">
+        <v>2</v>
+      </c>
+      <c r="Q177">
+        <v>0.5</v>
+      </c>
+      <c r="R177">
+        <v>1.8</v>
+      </c>
+      <c r="S177">
+        <v>2.05</v>
+      </c>
+      <c r="T177">
         <v>3</v>
       </c>
-      <c r="J177" t="s">
-        <v>43</v>
-      </c>
-      <c r="K177">
-        <v>4.2</v>
-      </c>
-      <c r="L177">
-        <v>3.75</v>
-      </c>
-      <c r="M177">
-        <v>1.8</v>
-      </c>
-      <c r="N177">
-        <v>4.75</v>
-      </c>
-      <c r="O177">
-        <v>4</v>
-      </c>
-      <c r="P177">
-        <v>1.7</v>
-      </c>
-      <c r="Q177">
-        <v>0.75</v>
-      </c>
-      <c r="R177">
-        <v>1.925</v>
-      </c>
-      <c r="S177">
-        <v>1.925</v>
-      </c>
-      <c r="T177">
-        <v>2.75</v>
-      </c>
       <c r="U177">
-        <v>1.975</v>
+        <v>2.025</v>
       </c>
       <c r="V177">
-        <v>1.875</v>
+        <v>1.825</v>
       </c>
       <c r="W177">
-        <v>-1</v>
+        <v>2.5</v>
       </c>
       <c r="X177">
         <v>-1</v>
       </c>
       <c r="Y177">
-        <v>0.7</v>
+        <v>-1</v>
       </c>
       <c r="Z177">
-        <v>-0.5</v>
+        <v>0.8</v>
       </c>
       <c r="AA177">
-        <v>0.4625</v>
+        <v>-1</v>
       </c>
       <c r="AB177">
-        <v>0.9750000000000001</v>
+        <v>-1</v>
       </c>
       <c r="AC177">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="178" spans="1:29">
@@ -16271,7 +16271,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>6847080</v>
+        <v>6847079</v>
       </c>
       <c r="C178" t="s">
         <v>28</v>
@@ -16283,76 +16283,76 @@
         <v>45241.54166666666</v>
       </c>
       <c r="F178" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G178" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="H178">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I178">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J178" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K178">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="L178">
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
       <c r="M178">
-        <v>2.15</v>
+        <v>1.8</v>
       </c>
       <c r="N178">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="O178">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="P178">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="Q178">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R178">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S178">
-        <v>2.05</v>
+        <v>1.925</v>
       </c>
       <c r="T178">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="U178">
-        <v>2.025</v>
+        <v>1.975</v>
       </c>
       <c r="V178">
-        <v>1.825</v>
+        <v>1.875</v>
       </c>
       <c r="W178">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X178">
         <v>-1</v>
       </c>
       <c r="Y178">
-        <v>-1</v>
+        <v>0.7</v>
       </c>
       <c r="Z178">
-        <v>0.8</v>
+        <v>-0.5</v>
       </c>
       <c r="AA178">
-        <v>-1</v>
+        <v>0.4625</v>
       </c>
       <c r="AB178">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AC178">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="179" spans="1:29">
@@ -16906,7 +16906,7 @@
         <v>45256.4375</v>
       </c>
       <c r="F185" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G185" t="s">
         <v>36</v>
@@ -17618,7 +17618,7 @@
         <v>45265.625</v>
       </c>
       <c r="F193" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G193" t="s">
         <v>37</v>
@@ -18155,7 +18155,7 @@
         <v>29</v>
       </c>
       <c r="G199" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H199">
         <v>1</v>
@@ -18295,6 +18295,154 @@
         <v>0</v>
       </c>
       <c r="AA200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:29">
+      <c r="A201" s="1">
+        <v>199</v>
+      </c>
+      <c r="B201">
+        <v>6851943</v>
+      </c>
+      <c r="C201" t="s">
+        <v>28</v>
+      </c>
+      <c r="D201" t="s">
+        <v>28</v>
+      </c>
+      <c r="E201" s="2">
+        <v>45332.54166666666</v>
+      </c>
+      <c r="F201" t="s">
+        <v>33</v>
+      </c>
+      <c r="G201" t="s">
+        <v>41</v>
+      </c>
+      <c r="K201">
+        <v>2.3</v>
+      </c>
+      <c r="L201">
+        <v>3.6</v>
+      </c>
+      <c r="M201">
+        <v>2.8</v>
+      </c>
+      <c r="N201">
+        <v>2.1</v>
+      </c>
+      <c r="O201">
+        <v>3.6</v>
+      </c>
+      <c r="P201">
+        <v>3.3</v>
+      </c>
+      <c r="Q201">
+        <v>-0.25</v>
+      </c>
+      <c r="R201">
+        <v>1.85</v>
+      </c>
+      <c r="S201">
+        <v>2</v>
+      </c>
+      <c r="T201">
+        <v>2.25</v>
+      </c>
+      <c r="U201">
+        <v>1.85</v>
+      </c>
+      <c r="V201">
+        <v>2</v>
+      </c>
+      <c r="W201">
+        <v>0</v>
+      </c>
+      <c r="X201">
+        <v>0</v>
+      </c>
+      <c r="Y201">
+        <v>0</v>
+      </c>
+      <c r="Z201">
+        <v>0</v>
+      </c>
+      <c r="AA201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:29">
+      <c r="A202" s="1">
+        <v>200</v>
+      </c>
+      <c r="B202">
+        <v>6847096</v>
+      </c>
+      <c r="C202" t="s">
+        <v>28</v>
+      </c>
+      <c r="D202" t="s">
+        <v>28</v>
+      </c>
+      <c r="E202" s="2">
+        <v>45332.54166666666</v>
+      </c>
+      <c r="F202" t="s">
+        <v>34</v>
+      </c>
+      <c r="G202" t="s">
+        <v>35</v>
+      </c>
+      <c r="K202">
+        <v>2</v>
+      </c>
+      <c r="L202">
+        <v>3.75</v>
+      </c>
+      <c r="M202">
+        <v>3.3</v>
+      </c>
+      <c r="N202">
+        <v>2.05</v>
+      </c>
+      <c r="O202">
+        <v>3.8</v>
+      </c>
+      <c r="P202">
+        <v>3.2</v>
+      </c>
+      <c r="Q202">
+        <v>-0.25</v>
+      </c>
+      <c r="R202">
+        <v>1.825</v>
+      </c>
+      <c r="S202">
+        <v>2.025</v>
+      </c>
+      <c r="T202">
+        <v>2.5</v>
+      </c>
+      <c r="U202">
+        <v>1.875</v>
+      </c>
+      <c r="V202">
+        <v>1.975</v>
+      </c>
+      <c r="W202">
+        <v>0</v>
+      </c>
+      <c r="X202">
+        <v>0</v>
+      </c>
+      <c r="Y202">
+        <v>0</v>
+      </c>
+      <c r="Z202">
+        <v>0</v>
+      </c>
+      <c r="AA202">
         <v>0</v>
       </c>
     </row>

</xml_diff>